<commit_message>
RE: AEP-DTAC- STM documents - Priority 1.2 as of 13-Apr-2020 request for review
For RBT_download_song_daily, the value in CUSTOMER_NUMBER column is MSISDN, privacy column marked in STM and added in ISD
</commit_message>
<xml_diff>
--- a/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.1.xlsx
+++ b/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telenor-AEP\Requirement-Docs\DTAC_STM_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telenor-AEP\Requirement-Docs\DTAC_Sprint1_SS_Feeds\IS_DTAC_Feeds\Review_Feb2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4047" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4049" uniqueCount="571">
   <si>
     <t>Mode of Integration</t>
   </si>
@@ -1774,6 +1774,9 @@
 1) DMS feeds
 2) other source feeds DIM,OMR,RBT,MD,MDD,CMPGN,ESRVC
 3)Discovery feeds shared in separate STM for review</t>
+  </si>
+  <si>
+    <t>encrypt(CUSTOMER_NUMBER)</t>
   </si>
 </sst>
 </file>
@@ -3053,13 +3056,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="32" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="35" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="34" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="32" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
@@ -3094,18 +3109,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="35" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -3426,7 +3429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D29" sqref="D29:F29"/>
     </sheetView>
   </sheetViews>
@@ -3448,12 +3451,12 @@
       <c r="A2" s="55"/>
     </row>
     <row r="3" spans="1:6" ht="20.25">
-      <c r="A3" s="210" t="s">
+      <c r="A3" s="214" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="210"/>
-      <c r="C3" s="210"/>
-      <c r="D3" s="210"/>
+      <c r="B3" s="214"/>
+      <c r="C3" s="214"/>
+      <c r="D3" s="214"/>
     </row>
     <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="55"/>
@@ -3477,10 +3480,10 @@
       <c r="F7" s="61"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="211" t="s">
+      <c r="A8" s="215" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="212"/>
+      <c r="B8" s="216"/>
       <c r="C8" s="62" t="s">
         <v>163</v>
       </c>
@@ -3507,7 +3510,7 @@
       <c r="F9" s="64"/>
     </row>
     <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="213" t="s">
+      <c r="A10" s="217" t="s">
         <v>169</v>
       </c>
       <c r="B10" s="66" t="s">
@@ -3519,7 +3522,7 @@
       <c r="F10" s="71"/>
     </row>
     <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="214"/>
+      <c r="A11" s="218"/>
       <c r="B11" s="72" t="s">
         <v>171</v>
       </c>
@@ -3549,7 +3552,7 @@
       <c r="F13" s="71"/>
     </row>
     <row r="14" spans="1:6" ht="15.75">
-      <c r="A14" s="215" t="s">
+      <c r="A14" s="219" t="s">
         <v>174</v>
       </c>
       <c r="B14" s="72" t="s">
@@ -3561,7 +3564,7 @@
       <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:6" ht="15.75">
-      <c r="A15" s="216"/>
+      <c r="A15" s="220"/>
       <c r="B15" s="66" t="s">
         <v>173</v>
       </c>
@@ -3571,7 +3574,7 @@
       <c r="F15" s="79"/>
     </row>
     <row r="16" spans="1:6" ht="15.75">
-      <c r="A16" s="216"/>
+      <c r="A16" s="220"/>
       <c r="B16" s="66" t="s">
         <v>176</v>
       </c>
@@ -3581,7 +3584,7 @@
       <c r="F16" s="79"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A17" s="217"/>
+      <c r="A17" s="221"/>
       <c r="B17" s="81" t="s">
         <v>177</v>
       </c>
@@ -3618,11 +3621,11 @@
       <c r="C20" s="88" t="s">
         <v>181</v>
       </c>
-      <c r="D20" s="218" t="s">
+      <c r="D20" s="222" t="s">
         <v>182</v>
       </c>
-      <c r="E20" s="219"/>
-      <c r="F20" s="220"/>
+      <c r="E20" s="223"/>
+      <c r="F20" s="224"/>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1">
       <c r="A21" s="89">
@@ -3634,11 +3637,11 @@
       <c r="C21" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="207" t="s">
+      <c r="D21" s="213" t="s">
         <v>184</v>
       </c>
-      <c r="E21" s="208"/>
-      <c r="F21" s="209"/>
+      <c r="E21" s="211"/>
+      <c r="F21" s="212"/>
     </row>
     <row r="22" spans="1:6" ht="36.75" customHeight="1">
       <c r="A22" s="92">
@@ -3650,11 +3653,11 @@
       <c r="C22" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D22" s="222" t="s">
+      <c r="D22" s="208" t="s">
         <v>186</v>
       </c>
-      <c r="E22" s="222"/>
-      <c r="F22" s="223"/>
+      <c r="E22" s="208"/>
+      <c r="F22" s="209"/>
     </row>
     <row r="23" spans="1:6" ht="31.5" customHeight="1">
       <c r="A23" s="92">
@@ -3666,11 +3669,11 @@
       <c r="C23" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D23" s="222" t="s">
+      <c r="D23" s="208" t="s">
         <v>187</v>
       </c>
-      <c r="E23" s="222"/>
-      <c r="F23" s="223"/>
+      <c r="E23" s="208"/>
+      <c r="F23" s="209"/>
     </row>
     <row r="24" spans="1:6" ht="44.25" customHeight="1">
       <c r="A24" s="92">
@@ -3682,11 +3685,11 @@
       <c r="C24" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D24" s="222" t="s">
+      <c r="D24" s="208" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="222"/>
-      <c r="F24" s="223"/>
+      <c r="E24" s="208"/>
+      <c r="F24" s="209"/>
     </row>
     <row r="25" spans="1:6" ht="89.25" customHeight="1">
       <c r="A25" s="92">
@@ -3698,11 +3701,11 @@
       <c r="C25" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D25" s="224" t="s">
+      <c r="D25" s="210" t="s">
         <v>189</v>
       </c>
-      <c r="E25" s="208"/>
-      <c r="F25" s="209"/>
+      <c r="E25" s="211"/>
+      <c r="F25" s="212"/>
     </row>
     <row r="26" spans="1:6" ht="44.25" customHeight="1">
       <c r="A26" s="92">
@@ -3714,11 +3717,11 @@
       <c r="C26" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D26" s="221" t="s">
+      <c r="D26" s="207" t="s">
         <v>190</v>
       </c>
-      <c r="E26" s="221"/>
-      <c r="F26" s="221"/>
+      <c r="E26" s="207"/>
+      <c r="F26" s="207"/>
     </row>
     <row r="27" spans="1:6" ht="44.25" customHeight="1">
       <c r="A27" s="92">
@@ -3730,11 +3733,11 @@
       <c r="C27" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="221" t="s">
+      <c r="D27" s="207" t="s">
         <v>191</v>
       </c>
-      <c r="E27" s="221"/>
-      <c r="F27" s="221"/>
+      <c r="E27" s="207"/>
+      <c r="F27" s="207"/>
     </row>
     <row r="28" spans="1:6" ht="44.25" customHeight="1">
       <c r="A28" s="92" t="s">
@@ -3746,11 +3749,11 @@
       <c r="C28" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="221" t="s">
+      <c r="D28" s="207" t="s">
         <v>193</v>
       </c>
-      <c r="E28" s="221"/>
-      <c r="F28" s="221"/>
+      <c r="E28" s="207"/>
+      <c r="F28" s="207"/>
     </row>
     <row r="29" spans="1:6" ht="54" customHeight="1">
       <c r="A29" s="92">
@@ -3762,14 +3765,20 @@
       <c r="C29" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D29" s="221" t="s">
+      <c r="D29" s="207" t="s">
         <v>569</v>
       </c>
-      <c r="E29" s="221"/>
-      <c r="F29" s="221"/>
+      <c r="E29" s="207"/>
+      <c r="F29" s="207"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D22:F22"/>
@@ -3778,12 +3787,6 @@
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -33369,7 +33372,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:V20"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -33386,7 +33389,7 @@
     <col min="10" max="11" width="16.140625" style="158" customWidth="1"/>
     <col min="12" max="12" width="7.7109375" customWidth="1"/>
     <col min="13" max="13" width="9" style="159" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" style="160" customWidth="1"/>
+    <col min="14" max="14" width="30.85546875" style="160" customWidth="1"/>
     <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" style="159" customWidth="1"/>
     <col min="17" max="17" width="17" style="159" bestFit="1" customWidth="1"/>
@@ -33464,7 +33467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:214" s="114" customFormat="1" ht="15" customHeight="1" collapsed="1">
+    <row r="2" spans="1:214" s="114" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="134" t="s">
         <v>22</v>
       </c>
@@ -33502,7 +33505,7 @@
       </c>
       <c r="R2" s="141" t="str">
         <f>IF(COUNTIF(R3:R12,"Y")&gt;0,"Y","N")</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
       <c r="S2" s="141" t="str">
         <f>IF(COUNTIF(S3:S12,"Y")&gt;0,"Y","N")</f>
@@ -33710,7 +33713,7 @@
       <c r="HE2" s="113"/>
       <c r="HF2" s="113"/>
     </row>
-    <row r="3" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="3" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A3" s="146" t="s">
         <v>22</v>
       </c>
@@ -33744,11 +33747,15 @@
       <c r="M3" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="123"/>
+      <c r="N3" s="123" t="s">
+        <v>570</v>
+      </c>
       <c r="O3" s="123"/>
       <c r="P3" s="147"/>
       <c r="Q3" s="147"/>
-      <c r="R3" s="147"/>
+      <c r="R3" s="147" t="s">
+        <v>32</v>
+      </c>
       <c r="S3" s="147"/>
       <c r="T3" s="147"/>
       <c r="U3" s="147"/>
@@ -33946,7 +33953,7 @@
       <c r="HE3" s="113"/>
       <c r="HF3" s="113"/>
     </row>
-    <row r="4" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="4" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A4" s="146" t="s">
         <v>22</v>
       </c>
@@ -34186,7 +34193,7 @@
       <c r="HE4" s="113"/>
       <c r="HF4" s="113"/>
     </row>
-    <row r="5" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="5" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A5" s="146" t="s">
         <v>22</v>
       </c>
@@ -34422,7 +34429,7 @@
       <c r="HE5" s="113"/>
       <c r="HF5" s="113"/>
     </row>
-    <row r="6" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="6" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A6" s="146" t="s">
         <v>22</v>
       </c>
@@ -34658,7 +34665,7 @@
       <c r="HE6" s="113"/>
       <c r="HF6" s="113"/>
     </row>
-    <row r="7" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="7" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A7" s="146" t="s">
         <v>22</v>
       </c>
@@ -34894,7 +34901,7 @@
       <c r="HE7" s="113"/>
       <c r="HF7" s="113"/>
     </row>
-    <row r="8" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="8" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A8" s="146" t="s">
         <v>22</v>
       </c>
@@ -35130,7 +35137,7 @@
       <c r="HE8" s="113"/>
       <c r="HF8" s="113"/>
     </row>
-    <row r="9" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="9" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A9" s="146" t="s">
         <v>22</v>
       </c>
@@ -35366,7 +35373,7 @@
       <c r="HE9" s="113"/>
       <c r="HF9" s="113"/>
     </row>
-    <row r="10" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="10" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A10" s="146" t="s">
         <v>22</v>
       </c>
@@ -35602,7 +35609,7 @@
       <c r="HE10" s="113"/>
       <c r="HF10" s="113"/>
     </row>
-    <row r="11" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="11" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A11" s="146" t="s">
         <v>22</v>
       </c>
@@ -35838,7 +35845,7 @@
       <c r="HE11" s="113"/>
       <c r="HF11" s="113"/>
     </row>
-    <row r="12" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="12" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A12" s="146" t="s">
         <v>22</v>
       </c>
@@ -36074,7 +36081,7 @@
       <c r="HE12" s="113"/>
       <c r="HF12" s="113"/>
     </row>
-    <row r="13" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="13" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A13" s="146" t="s">
         <v>22</v>
       </c>
@@ -36310,7 +36317,7 @@
       <c r="HE13" s="113"/>
       <c r="HF13" s="113"/>
     </row>
-    <row r="14" spans="1:214" s="122" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="14" spans="1:214" s="122" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A14" s="146" t="s">
         <v>22</v>
       </c>
@@ -36545,7 +36552,7 @@
       <c r="HE14" s="113"/>
       <c r="HF14" s="113"/>
     </row>
-    <row r="15" spans="1:214" s="113" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="15" spans="1:214" s="113" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A15" s="122"/>
       <c r="B15" s="121"/>
       <c r="C15" s="116"/>
@@ -36583,7 +36590,7 @@
       <c r="U15" s="120"/>
       <c r="V15" s="120"/>
     </row>
-    <row r="16" spans="1:214" s="113" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="16" spans="1:214" s="113" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A16" s="122"/>
       <c r="B16" s="121"/>
       <c r="C16" s="116"/>
@@ -36621,7 +36628,7 @@
       <c r="U16" s="120"/>
       <c r="V16" s="120"/>
     </row>
-    <row r="17" spans="1:22" s="113" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="17" spans="1:22" s="113" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A17" s="122"/>
       <c r="B17" s="121"/>
       <c r="C17" s="116"/>
@@ -36659,7 +36666,7 @@
       <c r="U17" s="120"/>
       <c r="V17" s="120"/>
     </row>
-    <row r="18" spans="1:22" s="113" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="18" spans="1:22" s="113" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A18" s="122"/>
       <c r="B18" s="121"/>
       <c r="C18" s="116"/>
@@ -36699,7 +36706,7 @@
       <c r="U18" s="120"/>
       <c r="V18" s="120"/>
     </row>
-    <row r="19" spans="1:22" s="113" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="19" spans="1:22" s="113" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A19" s="122"/>
       <c r="B19" s="121"/>
       <c r="C19" s="116"/>
@@ -36737,7 +36744,7 @@
       <c r="U19" s="120"/>
       <c r="V19" s="120"/>
     </row>
-    <row r="20" spans="1:22" s="113" customFormat="1" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="20" spans="1:22" s="113" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A20" s="122"/>
       <c r="B20" s="121"/>
       <c r="C20" s="122"/>
@@ -41459,7 +41466,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Arial"&amp;7 Sensitivity: Internal &amp; Restricted</oddFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Arial"&amp;7&amp;K000000Sensitivity: Internal &amp; Restricted</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -42188,6 +42195,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C723A6D629A244B9035064CEA29699F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="439c1f6a0871fabbc20469cf751fc22a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c6a5f84-dc80-404b-9608-a58c80d813cf" xmlns:ns3="fb15ab9c-5ce3-4966-97a0-841ffe55082a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a0ba7a63f3f3ddebd5188756dbc3799" ns2:_="" ns3:_="">
     <xsd:import namespace="5c6a5f84-dc80-404b-9608-a58c80d813cf"/>
@@ -42404,22 +42426,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6CC5F60-7C71-49F9-855C-F002D6759E81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86484D21-336C-4699-B297-37FD20E87A03}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D51A253-8FCC-480C-8849-892D45D1BD92}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42436,21 +42460,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86484D21-336C-4699-B297-37FD20E87A03}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6CC5F60-7C71-49F9-855C-F002D6759E81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[AEP - ODS] Change COMP_CD -> COMP_CODE for column from source file
</commit_message>
<xml_diff>
--- a/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.1.xlsx
+++ b/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Document - Sign-off" sheetId="4" r:id="rId1"/>
@@ -1524,9 +1524,6 @@
     <t xml:space="preserve">USSD_RESP_MSG                </t>
   </si>
   <si>
-    <t xml:space="preserve">COMP_CD                      </t>
-  </si>
-  <si>
     <t xml:space="preserve">REDEEM_TYPE                  </t>
   </si>
   <si>
@@ -1774,6 +1771,9 @@
   </si>
   <si>
     <t>encrypt(CUSTOMER_NUMBER)</t>
+  </si>
+  <si>
+    <t>COMP_CODE</t>
   </si>
 </sst>
 </file>
@@ -3053,13 +3053,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="32" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="35" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="34" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="32" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
@@ -3094,18 +3106,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="35" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -3448,12 +3448,12 @@
       <c r="A2" s="55"/>
     </row>
     <row r="3" spans="1:6" ht="20.25">
-      <c r="A3" s="210" t="s">
+      <c r="A3" s="214" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="210"/>
-      <c r="C3" s="210"/>
-      <c r="D3" s="210"/>
+      <c r="B3" s="214"/>
+      <c r="C3" s="214"/>
+      <c r="D3" s="214"/>
     </row>
     <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="55"/>
@@ -3477,10 +3477,10 @@
       <c r="F7" s="61"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="211" t="s">
+      <c r="A8" s="215" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="212"/>
+      <c r="B8" s="216"/>
       <c r="C8" s="62" t="s">
         <v>163</v>
       </c>
@@ -3507,7 +3507,7 @@
       <c r="F9" s="64"/>
     </row>
     <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="213" t="s">
+      <c r="A10" s="217" t="s">
         <v>169</v>
       </c>
       <c r="B10" s="66" t="s">
@@ -3519,7 +3519,7 @@
       <c r="F10" s="71"/>
     </row>
     <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="214"/>
+      <c r="A11" s="218"/>
       <c r="B11" s="72" t="s">
         <v>171</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="F13" s="71"/>
     </row>
     <row r="14" spans="1:6" ht="15.75">
-      <c r="A14" s="215" t="s">
+      <c r="A14" s="219" t="s">
         <v>174</v>
       </c>
       <c r="B14" s="72" t="s">
@@ -3561,7 +3561,7 @@
       <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:6" ht="15.75">
-      <c r="A15" s="216"/>
+      <c r="A15" s="220"/>
       <c r="B15" s="66" t="s">
         <v>173</v>
       </c>
@@ -3571,7 +3571,7 @@
       <c r="F15" s="79"/>
     </row>
     <row r="16" spans="1:6" ht="15.75">
-      <c r="A16" s="216"/>
+      <c r="A16" s="220"/>
       <c r="B16" s="66" t="s">
         <v>176</v>
       </c>
@@ -3581,7 +3581,7 @@
       <c r="F16" s="79"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A17" s="217"/>
+      <c r="A17" s="221"/>
       <c r="B17" s="81" t="s">
         <v>177</v>
       </c>
@@ -3618,11 +3618,11 @@
       <c r="C20" s="88" t="s">
         <v>181</v>
       </c>
-      <c r="D20" s="218" t="s">
+      <c r="D20" s="222" t="s">
         <v>182</v>
       </c>
-      <c r="E20" s="219"/>
-      <c r="F20" s="220"/>
+      <c r="E20" s="223"/>
+      <c r="F20" s="224"/>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1">
       <c r="A21" s="89">
@@ -3634,11 +3634,11 @@
       <c r="C21" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="207" t="s">
+      <c r="D21" s="213" t="s">
         <v>184</v>
       </c>
-      <c r="E21" s="208"/>
-      <c r="F21" s="209"/>
+      <c r="E21" s="211"/>
+      <c r="F21" s="212"/>
     </row>
     <row r="22" spans="1:6" ht="36.75" customHeight="1">
       <c r="A22" s="92">
@@ -3650,11 +3650,11 @@
       <c r="C22" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D22" s="222" t="s">
+      <c r="D22" s="208" t="s">
         <v>186</v>
       </c>
-      <c r="E22" s="222"/>
-      <c r="F22" s="223"/>
+      <c r="E22" s="208"/>
+      <c r="F22" s="209"/>
     </row>
     <row r="23" spans="1:6" ht="31.5" customHeight="1">
       <c r="A23" s="92">
@@ -3666,11 +3666,11 @@
       <c r="C23" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D23" s="222" t="s">
+      <c r="D23" s="208" t="s">
         <v>187</v>
       </c>
-      <c r="E23" s="222"/>
-      <c r="F23" s="223"/>
+      <c r="E23" s="208"/>
+      <c r="F23" s="209"/>
     </row>
     <row r="24" spans="1:6" ht="44.25" customHeight="1">
       <c r="A24" s="92">
@@ -3682,11 +3682,11 @@
       <c r="C24" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D24" s="222" t="s">
+      <c r="D24" s="208" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="222"/>
-      <c r="F24" s="223"/>
+      <c r="E24" s="208"/>
+      <c r="F24" s="209"/>
     </row>
     <row r="25" spans="1:6" ht="89.25" customHeight="1">
       <c r="A25" s="92">
@@ -3698,11 +3698,11 @@
       <c r="C25" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D25" s="224" t="s">
+      <c r="D25" s="210" t="s">
         <v>189</v>
       </c>
-      <c r="E25" s="208"/>
-      <c r="F25" s="209"/>
+      <c r="E25" s="211"/>
+      <c r="F25" s="212"/>
     </row>
     <row r="26" spans="1:6" ht="44.25" customHeight="1">
       <c r="A26" s="92">
@@ -3714,11 +3714,11 @@
       <c r="C26" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D26" s="221" t="s">
+      <c r="D26" s="207" t="s">
         <v>190</v>
       </c>
-      <c r="E26" s="221"/>
-      <c r="F26" s="221"/>
+      <c r="E26" s="207"/>
+      <c r="F26" s="207"/>
     </row>
     <row r="27" spans="1:6" ht="44.25" customHeight="1">
       <c r="A27" s="92">
@@ -3730,11 +3730,11 @@
       <c r="C27" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="221" t="s">
+      <c r="D27" s="207" t="s">
         <v>191</v>
       </c>
-      <c r="E27" s="221"/>
-      <c r="F27" s="221"/>
+      <c r="E27" s="207"/>
+      <c r="F27" s="207"/>
     </row>
     <row r="28" spans="1:6" ht="44.25" customHeight="1">
       <c r="A28" s="92" t="s">
@@ -3746,11 +3746,11 @@
       <c r="C28" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="221" t="s">
+      <c r="D28" s="207" t="s">
         <v>193</v>
       </c>
-      <c r="E28" s="221"/>
-      <c r="F28" s="221"/>
+      <c r="E28" s="207"/>
+      <c r="F28" s="207"/>
     </row>
     <row r="29" spans="1:6" ht="54" customHeight="1">
       <c r="A29" s="92">
@@ -3762,14 +3762,20 @@
       <c r="C29" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D29" s="221" t="s">
-        <v>568</v>
-      </c>
-      <c r="E29" s="221"/>
-      <c r="F29" s="221"/>
+      <c r="D29" s="207" t="s">
+        <v>567</v>
+      </c>
+      <c r="E29" s="207"/>
+      <c r="F29" s="207"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D22:F22"/>
@@ -3778,12 +3784,6 @@
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4754,7 +4754,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>23</v>
@@ -4805,7 +4805,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>23</v>
@@ -4851,7 +4851,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>23</v>
@@ -4895,7 +4895,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>23</v>
@@ -4939,7 +4939,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>23</v>
@@ -4983,7 +4983,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>23</v>
@@ -5027,7 +5027,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>23</v>
@@ -5071,7 +5071,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>23</v>
@@ -5119,7 +5119,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>23</v>
@@ -5163,7 +5163,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>23</v>
@@ -5442,7 +5442,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>23</v>
@@ -5493,7 +5493,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>23</v>
@@ -5539,7 +5539,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>23</v>
@@ -5583,7 +5583,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>23</v>
@@ -5627,7 +5627,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>23</v>
@@ -5671,7 +5671,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>23</v>
@@ -5715,7 +5715,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>23</v>
@@ -5759,7 +5759,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>23</v>
@@ -5803,7 +5803,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>23</v>
@@ -5851,7 +5851,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>23</v>
@@ -5899,7 +5899,7 @@
         <v>22</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>23</v>
@@ -6173,7 +6173,7 @@
         <v>22</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>23</v>
@@ -6224,7 +6224,7 @@
         <v>22</v>
       </c>
       <c r="B36" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C36" s="25" t="s">
         <v>23</v>
@@ -6268,7 +6268,7 @@
         <v>22</v>
       </c>
       <c r="B37" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>23</v>
@@ -6312,7 +6312,7 @@
         <v>22</v>
       </c>
       <c r="B38" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>23</v>
@@ -6356,7 +6356,7 @@
         <v>22</v>
       </c>
       <c r="B39" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C39" s="25" t="s">
         <v>23</v>
@@ -6402,7 +6402,7 @@
         <v>22</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C40" s="25" t="s">
         <v>23</v>
@@ -6446,7 +6446,7 @@
         <v>22</v>
       </c>
       <c r="B41" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C41" s="25" t="s">
         <v>23</v>
@@ -6490,7 +6490,7 @@
         <v>22</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C42" s="25" t="s">
         <v>23</v>
@@ -6534,7 +6534,7 @@
         <v>22</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C43" s="25" t="s">
         <v>23</v>
@@ -6578,7 +6578,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C44" s="25" t="s">
         <v>23</v>
@@ -6622,7 +6622,7 @@
         <v>22</v>
       </c>
       <c r="B45" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>23</v>
@@ -6666,7 +6666,7 @@
         <v>22</v>
       </c>
       <c r="B46" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C46" s="25" t="s">
         <v>23</v>
@@ -6710,7 +6710,7 @@
         <v>22</v>
       </c>
       <c r="B47" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C47" s="25" t="s">
         <v>23</v>
@@ -6754,7 +6754,7 @@
         <v>22</v>
       </c>
       <c r="B48" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C48" s="25" t="s">
         <v>23</v>
@@ -6798,7 +6798,7 @@
         <v>22</v>
       </c>
       <c r="B49" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C49" s="25" t="s">
         <v>23</v>
@@ -6842,7 +6842,7 @@
         <v>22</v>
       </c>
       <c r="B50" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>23</v>
@@ -6886,7 +6886,7 @@
         <v>22</v>
       </c>
       <c r="B51" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>23</v>
@@ -6930,7 +6930,7 @@
         <v>22</v>
       </c>
       <c r="B52" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C52" s="25" t="s">
         <v>23</v>
@@ -6974,7 +6974,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C53" s="25" t="s">
         <v>23</v>
@@ -7018,7 +7018,7 @@
         <v>22</v>
       </c>
       <c r="B54" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C54" s="25" t="s">
         <v>23</v>
@@ -7062,7 +7062,7 @@
         <v>22</v>
       </c>
       <c r="B55" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>23</v>
@@ -7106,7 +7106,7 @@
         <v>22</v>
       </c>
       <c r="B56" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>23</v>
@@ -7136,7 +7136,7 @@
         <v>32</v>
       </c>
       <c r="N56" s="24" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="O56" s="24"/>
       <c r="P56" s="204"/>
@@ -7154,7 +7154,7 @@
         <v>22</v>
       </c>
       <c r="B57" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C57" s="25" t="s">
         <v>23</v>
@@ -7184,7 +7184,7 @@
         <v>32</v>
       </c>
       <c r="N57" s="24" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="O57" s="24"/>
       <c r="P57" s="204"/>
@@ -7202,7 +7202,7 @@
         <v>22</v>
       </c>
       <c r="B58" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C58" s="25" t="s">
         <v>23</v>
@@ -7232,7 +7232,7 @@
         <v>32</v>
       </c>
       <c r="N58" s="24" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="O58" s="24"/>
       <c r="P58" s="204"/>
@@ -7250,7 +7250,7 @@
         <v>22</v>
       </c>
       <c r="B59" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>23</v>
@@ -7280,7 +7280,7 @@
         <v>32</v>
       </c>
       <c r="N59" s="24" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="O59" s="24"/>
       <c r="P59" s="204"/>
@@ -7298,7 +7298,7 @@
         <v>22</v>
       </c>
       <c r="B60" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>23</v>
@@ -7328,7 +7328,7 @@
         <v>32</v>
       </c>
       <c r="N60" s="24" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="O60" s="24"/>
       <c r="P60" s="204"/>
@@ -7346,13 +7346,13 @@
         <v>22</v>
       </c>
       <c r="B61" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D61" s="206" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
@@ -7361,7 +7361,7 @@
         <v>27</v>
       </c>
       <c r="I61" s="206" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J61" s="37" t="s">
         <v>62</v>
@@ -7390,13 +7390,13 @@
         <v>22</v>
       </c>
       <c r="B62" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D62" s="206" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
@@ -7405,7 +7405,7 @@
         <v>27</v>
       </c>
       <c r="I62" s="206" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J62" s="37" t="s">
         <v>62</v>
@@ -7434,7 +7434,7 @@
         <v>22</v>
       </c>
       <c r="B63" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>23</v>
@@ -7478,7 +7478,7 @@
         <v>22</v>
       </c>
       <c r="B64" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>23</v>
@@ -7522,7 +7522,7 @@
         <v>22</v>
       </c>
       <c r="B65" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C65" s="25" t="s">
         <v>23</v>
@@ -7570,7 +7570,7 @@
         <v>22</v>
       </c>
       <c r="B66" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>23</v>
@@ -7614,7 +7614,7 @@
         <v>22</v>
       </c>
       <c r="B67" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C67" s="25" t="s">
         <v>23</v>
@@ -7662,7 +7662,7 @@
         <v>22</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>23</v>
@@ -7710,7 +7710,7 @@
         <v>22</v>
       </c>
       <c r="B69" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C69" s="25" t="s">
         <v>23</v>
@@ -7758,7 +7758,7 @@
         <v>22</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C70" s="25" t="s">
         <v>23</v>
@@ -7802,7 +7802,7 @@
         <v>22</v>
       </c>
       <c r="B71" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C71" s="25" t="s">
         <v>23</v>
@@ -7846,7 +7846,7 @@
         <v>22</v>
       </c>
       <c r="B72" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C72" s="25" t="s">
         <v>23</v>
@@ -7894,7 +7894,7 @@
         <v>22</v>
       </c>
       <c r="B73" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C73" s="25" t="s">
         <v>23</v>
@@ -7938,7 +7938,7 @@
         <v>22</v>
       </c>
       <c r="B74" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C74" s="25" t="s">
         <v>23</v>
@@ -7982,7 +7982,7 @@
         <v>22</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C75" s="25" t="s">
         <v>23</v>
@@ -8256,7 +8256,7 @@
         <v>22</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C82" s="19" t="s">
         <v>23</v>
@@ -8307,7 +8307,7 @@
         <v>22</v>
       </c>
       <c r="B83" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C83" s="26" t="s">
         <v>23</v>
@@ -8353,7 +8353,7 @@
         <v>22</v>
       </c>
       <c r="B84" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C84" s="26" t="s">
         <v>23</v>
@@ -8397,7 +8397,7 @@
         <v>22</v>
       </c>
       <c r="B85" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C85" s="26" t="s">
         <v>23</v>
@@ -8441,7 +8441,7 @@
         <v>22</v>
       </c>
       <c r="B86" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C86" s="26" t="s">
         <v>23</v>
@@ -8485,7 +8485,7 @@
         <v>22</v>
       </c>
       <c r="B87" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C87" s="26" t="s">
         <v>23</v>
@@ -8529,7 +8529,7 @@
         <v>22</v>
       </c>
       <c r="B88" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C88" s="26" t="s">
         <v>23</v>
@@ -8573,7 +8573,7 @@
         <v>22</v>
       </c>
       <c r="B89" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C89" s="26" t="s">
         <v>23</v>
@@ -8617,7 +8617,7 @@
         <v>22</v>
       </c>
       <c r="B90" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C90" s="26" t="s">
         <v>23</v>
@@ -8665,7 +8665,7 @@
         <v>22</v>
       </c>
       <c r="B91" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C91" s="26" t="s">
         <v>23</v>
@@ -8709,7 +8709,7 @@
         <v>22</v>
       </c>
       <c r="B92" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C92" s="26" t="s">
         <v>23</v>
@@ -8987,7 +8987,7 @@
         <v>22</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C99" s="9" t="s">
         <v>23</v>
@@ -9038,7 +9038,7 @@
         <v>22</v>
       </c>
       <c r="B100" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C100" s="26" t="s">
         <v>23</v>
@@ -9084,7 +9084,7 @@
         <v>22</v>
       </c>
       <c r="B101" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C101" s="26" t="s">
         <v>23</v>
@@ -9128,7 +9128,7 @@
         <v>22</v>
       </c>
       <c r="B102" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C102" s="26" t="s">
         <v>23</v>
@@ -9172,7 +9172,7 @@
         <v>22</v>
       </c>
       <c r="B103" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C103" s="26" t="s">
         <v>23</v>
@@ -9216,7 +9216,7 @@
         <v>22</v>
       </c>
       <c r="B104" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C104" s="26" t="s">
         <v>23</v>
@@ -9260,7 +9260,7 @@
         <v>22</v>
       </c>
       <c r="B105" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C105" s="26" t="s">
         <v>23</v>
@@ -9304,7 +9304,7 @@
         <v>22</v>
       </c>
       <c r="B106" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C106" s="26" t="s">
         <v>23</v>
@@ -9348,7 +9348,7 @@
         <v>22</v>
       </c>
       <c r="B107" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C107" s="26" t="s">
         <v>23</v>
@@ -9392,7 +9392,7 @@
         <v>22</v>
       </c>
       <c r="B108" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C108" s="26" t="s">
         <v>23</v>
@@ -9436,7 +9436,7 @@
         <v>22</v>
       </c>
       <c r="B109" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C109" s="26" t="s">
         <v>23</v>
@@ -9480,7 +9480,7 @@
         <v>22</v>
       </c>
       <c r="B110" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C110" s="26" t="s">
         <v>23</v>
@@ -9524,7 +9524,7 @@
         <v>22</v>
       </c>
       <c r="B111" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C111" s="26" t="s">
         <v>23</v>
@@ -9568,7 +9568,7 @@
         <v>22</v>
       </c>
       <c r="B112" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C112" s="26" t="s">
         <v>23</v>
@@ -9612,7 +9612,7 @@
         <v>22</v>
       </c>
       <c r="B113" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C113" s="26" t="s">
         <v>23</v>
@@ -9656,7 +9656,7 @@
         <v>22</v>
       </c>
       <c r="B114" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C114" s="26" t="s">
         <v>23</v>
@@ -9700,7 +9700,7 @@
         <v>22</v>
       </c>
       <c r="B115" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C115" s="26" t="s">
         <v>23</v>
@@ -9744,7 +9744,7 @@
         <v>22</v>
       </c>
       <c r="B116" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C116" s="26" t="s">
         <v>23</v>
@@ -9788,7 +9788,7 @@
         <v>22</v>
       </c>
       <c r="B117" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C117" s="26" t="s">
         <v>23</v>
@@ -9832,7 +9832,7 @@
         <v>22</v>
       </c>
       <c r="B118" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C118" s="26" t="s">
         <v>23</v>
@@ -9876,7 +9876,7 @@
         <v>22</v>
       </c>
       <c r="B119" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C119" s="26" t="s">
         <v>23</v>
@@ -9920,7 +9920,7 @@
         <v>22</v>
       </c>
       <c r="B120" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C120" s="26" t="s">
         <v>23</v>
@@ -9964,7 +9964,7 @@
         <v>22</v>
       </c>
       <c r="B121" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C121" s="26" t="s">
         <v>23</v>
@@ -10008,7 +10008,7 @@
         <v>22</v>
       </c>
       <c r="B122" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C122" s="26" t="s">
         <v>23</v>
@@ -10052,7 +10052,7 @@
         <v>22</v>
       </c>
       <c r="B123" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C123" s="26" t="s">
         <v>23</v>
@@ -10096,7 +10096,7 @@
         <v>22</v>
       </c>
       <c r="B124" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C124" s="26" t="s">
         <v>23</v>
@@ -10144,7 +10144,7 @@
         <v>22</v>
       </c>
       <c r="B125" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C125" s="26" t="s">
         <v>23</v>
@@ -10188,7 +10188,7 @@
         <v>22</v>
       </c>
       <c r="B126" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C126" s="26" t="s">
         <v>23</v>
@@ -10232,7 +10232,7 @@
         <v>22</v>
       </c>
       <c r="B127" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C127" s="26" t="s">
         <v>23</v>
@@ -10276,7 +10276,7 @@
         <v>22</v>
       </c>
       <c r="B128" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C128" s="26" t="s">
         <v>23</v>
@@ -10320,7 +10320,7 @@
         <v>22</v>
       </c>
       <c r="B129" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C129" s="26" t="s">
         <v>23</v>
@@ -10368,7 +10368,7 @@
         <v>22</v>
       </c>
       <c r="B130" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C130" s="26" t="s">
         <v>23</v>
@@ -10412,7 +10412,7 @@
         <v>22</v>
       </c>
       <c r="B131" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C131" s="26" t="s">
         <v>23</v>
@@ -10709,7 +10709,7 @@
   </sheetPr>
   <dimension ref="A1:HF48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -10825,7 +10825,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="137" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I2" s="137"/>
       <c r="J2" s="140"/>
@@ -11069,7 +11069,7 @@
       <c r="F3" s="123"/>
       <c r="G3" s="123"/>
       <c r="H3" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I3" s="123" t="s">
         <v>288</v>
@@ -11307,7 +11307,7 @@
       <c r="F4" s="123"/>
       <c r="G4" s="123"/>
       <c r="H4" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I4" s="123" t="s">
         <v>289</v>
@@ -11543,7 +11543,7 @@
       <c r="F5" s="123"/>
       <c r="G5" s="123"/>
       <c r="H5" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I5" s="123" t="s">
         <v>290</v>
@@ -11779,7 +11779,7 @@
       <c r="F6" s="123"/>
       <c r="G6" s="123"/>
       <c r="H6" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I6" s="123" t="s">
         <v>291</v>
@@ -12015,7 +12015,7 @@
       <c r="F7" s="123"/>
       <c r="G7" s="123"/>
       <c r="H7" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I7" s="123" t="s">
         <v>292</v>
@@ -12251,7 +12251,7 @@
       <c r="F8" s="123"/>
       <c r="G8" s="123"/>
       <c r="H8" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I8" s="123" t="s">
         <v>293</v>
@@ -12487,7 +12487,7 @@
       <c r="F9" s="123"/>
       <c r="G9" s="123"/>
       <c r="H9" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I9" s="123" t="s">
         <v>294</v>
@@ -12723,7 +12723,7 @@
       <c r="F10" s="123"/>
       <c r="G10" s="123"/>
       <c r="H10" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I10" s="123" t="s">
         <v>295</v>
@@ -12959,7 +12959,7 @@
       <c r="F11" s="123"/>
       <c r="G11" s="123"/>
       <c r="H11" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I11" s="123" t="s">
         <v>296</v>
@@ -13195,7 +13195,7 @@
       <c r="F12" s="123"/>
       <c r="G12" s="123"/>
       <c r="H12" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I12" s="123" t="s">
         <v>297</v>
@@ -13431,7 +13431,7 @@
       <c r="F13" s="123"/>
       <c r="G13" s="123"/>
       <c r="H13" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I13" s="123" t="s">
         <v>298</v>
@@ -13667,7 +13667,7 @@
       <c r="F14" s="123"/>
       <c r="G14" s="123"/>
       <c r="H14" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I14" s="123" t="s">
         <v>299</v>
@@ -13902,7 +13902,7 @@
       <c r="F15" s="123"/>
       <c r="G15" s="123"/>
       <c r="H15" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I15" s="123" t="s">
         <v>300</v>
@@ -14137,7 +14137,7 @@
       <c r="F16" s="123"/>
       <c r="G16" s="123"/>
       <c r="H16" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I16" s="123" t="s">
         <v>301</v>
@@ -14373,7 +14373,7 @@
       <c r="F17" s="123"/>
       <c r="G17" s="123"/>
       <c r="H17" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I17" s="123" t="s">
         <v>302</v>
@@ -14609,7 +14609,7 @@
       <c r="F18" s="123"/>
       <c r="G18" s="123"/>
       <c r="H18" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I18" s="123" t="s">
         <v>303</v>
@@ -14845,7 +14845,7 @@
       <c r="F19" s="123"/>
       <c r="G19" s="123"/>
       <c r="H19" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I19" s="123" t="s">
         <v>304</v>
@@ -15081,7 +15081,7 @@
       <c r="F20" s="123"/>
       <c r="G20" s="123"/>
       <c r="H20" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I20" s="123" t="s">
         <v>305</v>
@@ -15317,7 +15317,7 @@
       <c r="F21" s="123"/>
       <c r="G21" s="123"/>
       <c r="H21" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I21" s="123" t="s">
         <v>306</v>
@@ -15553,7 +15553,7 @@
       <c r="F22" s="123"/>
       <c r="G22" s="123"/>
       <c r="H22" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I22" s="123" t="s">
         <v>307</v>
@@ -15789,7 +15789,7 @@
       <c r="F23" s="123"/>
       <c r="G23" s="123"/>
       <c r="H23" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I23" s="123" t="s">
         <v>308</v>
@@ -16025,7 +16025,7 @@
       <c r="F24" s="123"/>
       <c r="G24" s="123"/>
       <c r="H24" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I24" s="123" t="s">
         <v>309</v>
@@ -16260,7 +16260,7 @@
       <c r="F25" s="123"/>
       <c r="G25" s="123"/>
       <c r="H25" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I25" s="123" t="s">
         <v>310</v>
@@ -16495,7 +16495,7 @@
       <c r="F26" s="123"/>
       <c r="G26" s="123"/>
       <c r="H26" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I26" s="123" t="s">
         <v>311</v>
@@ -16731,7 +16731,7 @@
       <c r="F27" s="123"/>
       <c r="G27" s="123"/>
       <c r="H27" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I27" s="123" t="s">
         <v>312</v>
@@ -16967,7 +16967,7 @@
       <c r="F28" s="123"/>
       <c r="G28" s="123"/>
       <c r="H28" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I28" s="123" t="s">
         <v>313</v>
@@ -17203,7 +17203,7 @@
       <c r="F29" s="123"/>
       <c r="G29" s="123"/>
       <c r="H29" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I29" s="123" t="s">
         <v>314</v>
@@ -17439,7 +17439,7 @@
       <c r="F30" s="123"/>
       <c r="G30" s="123"/>
       <c r="H30" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I30" s="123" t="s">
         <v>315</v>
@@ -17675,7 +17675,7 @@
       <c r="F31" s="123"/>
       <c r="G31" s="123"/>
       <c r="H31" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I31" s="123" t="s">
         <v>316</v>
@@ -17911,7 +17911,7 @@
       <c r="F32" s="123"/>
       <c r="G32" s="123"/>
       <c r="H32" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I32" s="123" t="s">
         <v>317</v>
@@ -18147,7 +18147,7 @@
       <c r="F33" s="123"/>
       <c r="G33" s="123"/>
       <c r="H33" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I33" s="123" t="s">
         <v>318</v>
@@ -18191,7 +18191,7 @@
       <c r="F34" s="123"/>
       <c r="G34" s="123"/>
       <c r="H34" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I34" s="123" t="s">
         <v>319</v>
@@ -18235,7 +18235,7 @@
       <c r="F35" s="123"/>
       <c r="G35" s="123"/>
       <c r="H35" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I35" s="123" t="s">
         <v>320</v>
@@ -18471,7 +18471,7 @@
       <c r="F36" s="123"/>
       <c r="G36" s="123"/>
       <c r="H36" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I36" s="123" t="s">
         <v>321</v>
@@ -18707,7 +18707,7 @@
       <c r="F37" s="123"/>
       <c r="G37" s="123"/>
       <c r="H37" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I37" s="123" t="s">
         <v>322</v>
@@ -18943,7 +18943,7 @@
       <c r="F38" s="123"/>
       <c r="G38" s="123"/>
       <c r="H38" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I38" s="123" t="s">
         <v>323</v>
@@ -19179,7 +19179,7 @@
       <c r="F39" s="123"/>
       <c r="G39" s="123"/>
       <c r="H39" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I39" s="123" t="s">
         <v>324</v>
@@ -19415,7 +19415,7 @@
       <c r="F40" s="123"/>
       <c r="G40" s="123"/>
       <c r="H40" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I40" s="123" t="s">
         <v>325</v>
@@ -19651,7 +19651,7 @@
       <c r="F41" s="123"/>
       <c r="G41" s="123"/>
       <c r="H41" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I41" s="123" t="s">
         <v>326</v>
@@ -19887,7 +19887,7 @@
       <c r="F42" s="123"/>
       <c r="G42" s="123"/>
       <c r="H42" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I42" s="123" t="s">
         <v>327</v>
@@ -19925,7 +19925,7 @@
       <c r="F43" s="116"/>
       <c r="G43" s="116"/>
       <c r="H43" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I43" s="150" t="s">
         <v>51</v>
@@ -19963,7 +19963,7 @@
       <c r="F44" s="116"/>
       <c r="G44" s="116"/>
       <c r="H44" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I44" s="124" t="s">
         <v>52</v>
@@ -20001,7 +20001,7 @@
       <c r="F45" s="116"/>
       <c r="G45" s="116"/>
       <c r="H45" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I45" s="124" t="s">
         <v>53</v>
@@ -20039,7 +20039,7 @@
       <c r="F46" s="116"/>
       <c r="G46" s="116"/>
       <c r="H46" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I46" s="124" t="s">
         <v>54</v>
@@ -20079,7 +20079,7 @@
       <c r="F47" s="116"/>
       <c r="G47" s="116"/>
       <c r="H47" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I47" s="124" t="s">
         <v>55</v>
@@ -20115,7 +20115,7 @@
       <c r="F48" s="122"/>
       <c r="G48" s="122"/>
       <c r="H48" s="123" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I48" s="124" t="s">
         <v>56</v>
@@ -20520,7 +20520,7 @@
         <v>418</v>
       </c>
       <c r="J3" s="171" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K3" s="123"/>
       <c r="L3" s="171" t="s">
@@ -20530,7 +20530,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="124" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="O3" s="124"/>
       <c r="P3" s="126"/>
@@ -22702,7 +22702,7 @@
         <v>32</v>
       </c>
       <c r="N13" s="123" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="O13" s="123"/>
       <c r="P13" s="147"/>
@@ -22942,7 +22942,7 @@
         <v>32</v>
       </c>
       <c r="N14" s="123" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O14" s="123"/>
       <c r="P14" s="147"/>
@@ -26498,7 +26498,7 @@
         <v>32</v>
       </c>
       <c r="N29" s="123" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="O29" s="123"/>
       <c r="P29" s="147"/>
@@ -26974,7 +26974,7 @@
         <v>32</v>
       </c>
       <c r="N31" s="123" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O31" s="123"/>
       <c r="P31" s="147"/>
@@ -27214,7 +27214,7 @@
         <v>32</v>
       </c>
       <c r="N32" s="123" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="O32" s="123"/>
       <c r="P32" s="147"/>
@@ -33745,7 +33745,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="123" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="O3" s="123"/>
       <c r="P3" s="147"/>
@@ -36797,10 +36797,10 @@
   </sheetPr>
   <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -36902,10 +36902,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="193" t="s">
+        <v>556</v>
+      </c>
+      <c r="C2" s="163" t="s">
         <v>557</v>
-      </c>
-      <c r="C2" s="163" t="s">
-        <v>558</v>
       </c>
       <c r="D2" s="164"/>
       <c r="E2" s="164"/>
@@ -36916,7 +36916,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="165" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I2" s="162"/>
       <c r="J2" s="162"/>
@@ -36962,13 +36962,13 @@
       <c r="F3" s="124"/>
       <c r="G3" s="124"/>
       <c r="H3" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I3" s="171" t="s">
         <v>418</v>
       </c>
       <c r="J3" s="171" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K3" s="171"/>
       <c r="L3" s="172" t="s">
@@ -36978,7 +36978,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="124" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="O3" s="124"/>
       <c r="P3" s="126"/>
@@ -36996,30 +36996,30 @@
         <v>22</v>
       </c>
       <c r="B4" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C4" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C4" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D4" s="123" t="s">
         <v>451</v>
       </c>
       <c r="E4" s="192" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F4" s="124"/>
       <c r="G4" s="124"/>
       <c r="H4" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I4" s="123" t="s">
         <v>451</v>
       </c>
       <c r="J4" s="123" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K4" s="123" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L4" s="172" t="s">
         <v>59</v>
@@ -37028,7 +37028,7 @@
         <v>32</v>
       </c>
       <c r="N4" s="192" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="O4" s="124"/>
       <c r="P4" s="126"/>
@@ -37044,10 +37044,10 @@
         <v>22</v>
       </c>
       <c r="B5" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C5" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C5" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D5" s="123" t="s">
         <v>452</v>
@@ -37056,7 +37056,7 @@
       <c r="F5" s="124"/>
       <c r="G5" s="124"/>
       <c r="H5" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I5" s="123" t="s">
         <v>452</v>
@@ -37086,10 +37086,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C6" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C6" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D6" s="123" t="s">
         <v>453</v>
@@ -37098,7 +37098,7 @@
       <c r="F6" s="124"/>
       <c r="G6" s="124"/>
       <c r="H6" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I6" s="123" t="s">
         <v>453</v>
@@ -37116,7 +37116,7 @@
         <v>32</v>
       </c>
       <c r="N6" s="124" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="O6" s="124"/>
       <c r="P6" s="126"/>
@@ -37134,10 +37134,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C7" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C7" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D7" s="123" t="s">
         <v>454</v>
@@ -37146,7 +37146,7 @@
       <c r="F7" s="124"/>
       <c r="G7" s="124"/>
       <c r="H7" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I7" s="123" t="s">
         <v>454</v>
@@ -37178,10 +37178,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C8" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C8" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D8" s="123" t="s">
         <v>455</v>
@@ -37190,7 +37190,7 @@
       <c r="F8" s="124"/>
       <c r="G8" s="124"/>
       <c r="H8" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I8" s="123" t="s">
         <v>455</v>
@@ -37222,10 +37222,10 @@
         <v>22</v>
       </c>
       <c r="B9" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C9" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C9" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D9" s="123" t="s">
         <v>456</v>
@@ -37234,7 +37234,7 @@
       <c r="F9" s="124"/>
       <c r="G9" s="124"/>
       <c r="H9" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I9" s="123" t="s">
         <v>456</v>
@@ -37266,10 +37266,10 @@
         <v>22</v>
       </c>
       <c r="B10" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C10" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C10" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D10" s="123" t="s">
         <v>457</v>
@@ -37278,7 +37278,7 @@
       <c r="F10" s="124"/>
       <c r="G10" s="124"/>
       <c r="H10" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I10" s="123" t="s">
         <v>457</v>
@@ -37310,30 +37310,30 @@
         <v>22</v>
       </c>
       <c r="B11" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C11" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C11" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D11" s="123" t="s">
         <v>458</v>
       </c>
       <c r="E11" s="192" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F11" s="124"/>
       <c r="G11" s="124"/>
       <c r="H11" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I11" s="123" t="s">
         <v>458</v>
       </c>
       <c r="J11" s="123" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K11" s="123" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L11" s="172" t="s">
         <v>59</v>
@@ -37342,7 +37342,7 @@
         <v>32</v>
       </c>
       <c r="N11" s="192" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="O11" s="124"/>
       <c r="P11" s="126"/>
@@ -37358,30 +37358,30 @@
         <v>22</v>
       </c>
       <c r="B12" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C12" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C12" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D12" s="123" t="s">
         <v>459</v>
       </c>
       <c r="E12" s="192" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F12" s="124"/>
       <c r="G12" s="124"/>
       <c r="H12" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I12" s="123" t="s">
         <v>459</v>
       </c>
       <c r="J12" s="123" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K12" s="123" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L12" s="172" t="s">
         <v>59</v>
@@ -37390,7 +37390,7 @@
         <v>32</v>
       </c>
       <c r="N12" s="192" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="O12" s="124"/>
       <c r="P12" s="126"/>
@@ -37406,10 +37406,10 @@
         <v>22</v>
       </c>
       <c r="B13" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C13" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C13" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D13" s="123" t="s">
         <v>460</v>
@@ -37418,7 +37418,7 @@
       <c r="F13" s="124"/>
       <c r="G13" s="124"/>
       <c r="H13" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I13" s="123" t="s">
         <v>460</v>
@@ -37450,10 +37450,10 @@
         <v>22</v>
       </c>
       <c r="B14" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C14" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C14" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D14" s="123" t="s">
         <v>461</v>
@@ -37462,7 +37462,7 @@
       <c r="F14" s="124"/>
       <c r="G14" s="124"/>
       <c r="H14" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I14" s="123" t="s">
         <v>461</v>
@@ -37494,10 +37494,10 @@
         <v>22</v>
       </c>
       <c r="B15" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C15" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C15" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D15" s="123" t="s">
         <v>462</v>
@@ -37506,7 +37506,7 @@
       <c r="F15" s="124"/>
       <c r="G15" s="124"/>
       <c r="H15" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I15" s="123" t="s">
         <v>462</v>
@@ -37538,10 +37538,10 @@
         <v>22</v>
       </c>
       <c r="B16" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C16" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C16" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D16" s="123" t="s">
         <v>463</v>
@@ -37550,7 +37550,7 @@
       <c r="F16" s="124"/>
       <c r="G16" s="124"/>
       <c r="H16" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I16" s="123" t="s">
         <v>463</v>
@@ -37582,10 +37582,10 @@
         <v>22</v>
       </c>
       <c r="B17" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C17" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C17" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D17" s="123" t="s">
         <v>464</v>
@@ -37594,7 +37594,7 @@
       <c r="F17" s="124"/>
       <c r="G17" s="124"/>
       <c r="H17" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I17" s="123" t="s">
         <v>464</v>
@@ -37626,10 +37626,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C18" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C18" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D18" s="123" t="s">
         <v>465</v>
@@ -37638,7 +37638,7 @@
       <c r="F18" s="124"/>
       <c r="G18" s="124"/>
       <c r="H18" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I18" s="123" t="s">
         <v>465</v>
@@ -37670,10 +37670,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C19" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C19" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D19" s="123" t="s">
         <v>466</v>
@@ -37682,7 +37682,7 @@
       <c r="F19" s="124"/>
       <c r="G19" s="124"/>
       <c r="H19" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I19" s="123" t="s">
         <v>466</v>
@@ -37714,10 +37714,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C20" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C20" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D20" s="123" t="s">
         <v>467</v>
@@ -37726,16 +37726,16 @@
       <c r="F20" s="124"/>
       <c r="G20" s="124"/>
       <c r="H20" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I20" s="123" t="s">
         <v>467</v>
       </c>
       <c r="J20" s="123" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K20" s="123" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L20" s="172" t="s">
         <v>59</v>
@@ -37758,10 +37758,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C21" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C21" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D21" s="123" t="s">
         <v>468</v>
@@ -37770,7 +37770,7 @@
       <c r="F21" s="124"/>
       <c r="G21" s="124"/>
       <c r="H21" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I21" s="123" t="s">
         <v>468</v>
@@ -37802,10 +37802,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C22" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C22" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D22" s="123" t="s">
         <v>469</v>
@@ -37814,7 +37814,7 @@
       <c r="F22" s="124"/>
       <c r="G22" s="124"/>
       <c r="H22" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I22" s="123" t="s">
         <v>469</v>
@@ -37846,10 +37846,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C23" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C23" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D23" s="123" t="s">
         <v>470</v>
@@ -37858,7 +37858,7 @@
       <c r="F23" s="124"/>
       <c r="G23" s="124"/>
       <c r="H23" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I23" s="123" t="s">
         <v>470</v>
@@ -37890,10 +37890,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C24" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C24" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D24" s="123" t="s">
         <v>471</v>
@@ -37902,16 +37902,16 @@
       <c r="F24" s="124"/>
       <c r="G24" s="124"/>
       <c r="H24" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I24" s="123" t="s">
         <v>471</v>
       </c>
       <c r="J24" s="123" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K24" s="123" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L24" s="172" t="s">
         <v>59</v>
@@ -37934,10 +37934,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C25" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C25" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D25" s="123" t="s">
         <v>472</v>
@@ -37946,7 +37946,7 @@
       <c r="F25" s="124"/>
       <c r="G25" s="124"/>
       <c r="H25" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I25" s="123" t="s">
         <v>472</v>
@@ -37978,10 +37978,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C26" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C26" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D26" s="123" t="s">
         <v>473</v>
@@ -37990,7 +37990,7 @@
       <c r="F26" s="124"/>
       <c r="G26" s="124"/>
       <c r="H26" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I26" s="123" t="s">
         <v>473</v>
@@ -38022,10 +38022,10 @@
         <v>22</v>
       </c>
       <c r="B27" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C27" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C27" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D27" s="123" t="s">
         <v>474</v>
@@ -38034,7 +38034,7 @@
       <c r="F27" s="124"/>
       <c r="G27" s="124"/>
       <c r="H27" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I27" s="123" t="s">
         <v>474</v>
@@ -38066,10 +38066,10 @@
         <v>22</v>
       </c>
       <c r="B28" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C28" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C28" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D28" s="123" t="s">
         <v>475</v>
@@ -38078,7 +38078,7 @@
       <c r="F28" s="124"/>
       <c r="G28" s="124"/>
       <c r="H28" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I28" s="123" t="s">
         <v>475</v>
@@ -38110,10 +38110,10 @@
         <v>22</v>
       </c>
       <c r="B29" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C29" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C29" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D29" s="123" t="s">
         <v>476</v>
@@ -38122,7 +38122,7 @@
       <c r="F29" s="124"/>
       <c r="G29" s="124"/>
       <c r="H29" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I29" s="123" t="s">
         <v>476</v>
@@ -38154,10 +38154,10 @@
         <v>22</v>
       </c>
       <c r="B30" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C30" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C30" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D30" s="123" t="s">
         <v>477</v>
@@ -38166,7 +38166,7 @@
       <c r="F30" s="124"/>
       <c r="G30" s="124"/>
       <c r="H30" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I30" s="123" t="s">
         <v>477</v>
@@ -38198,10 +38198,10 @@
         <v>22</v>
       </c>
       <c r="B31" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C31" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C31" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D31" s="123" t="s">
         <v>478</v>
@@ -38210,7 +38210,7 @@
       <c r="F31" s="124"/>
       <c r="G31" s="124"/>
       <c r="H31" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I31" s="123" t="s">
         <v>478</v>
@@ -38242,10 +38242,10 @@
         <v>22</v>
       </c>
       <c r="B32" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C32" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C32" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D32" s="123" t="s">
         <v>479</v>
@@ -38254,7 +38254,7 @@
       <c r="F32" s="124"/>
       <c r="G32" s="124"/>
       <c r="H32" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I32" s="123" t="s">
         <v>479</v>
@@ -38286,10 +38286,10 @@
         <v>22</v>
       </c>
       <c r="B33" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C33" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C33" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D33" s="123" t="s">
         <v>480</v>
@@ -38298,7 +38298,7 @@
       <c r="F33" s="124"/>
       <c r="G33" s="124"/>
       <c r="H33" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I33" s="123" t="s">
         <v>480</v>
@@ -38330,10 +38330,10 @@
         <v>22</v>
       </c>
       <c r="B34" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C34" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C34" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D34" s="123" t="s">
         <v>481</v>
@@ -38342,7 +38342,7 @@
       <c r="F34" s="124"/>
       <c r="G34" s="124"/>
       <c r="H34" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I34" s="123" t="s">
         <v>481</v>
@@ -38374,10 +38374,10 @@
         <v>22</v>
       </c>
       <c r="B35" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C35" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C35" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D35" s="123" t="s">
         <v>482</v>
@@ -38386,7 +38386,7 @@
       <c r="F35" s="124"/>
       <c r="G35" s="124"/>
       <c r="H35" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I35" s="123" t="s">
         <v>482</v>
@@ -38418,10 +38418,10 @@
         <v>22</v>
       </c>
       <c r="B36" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C36" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C36" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D36" s="123" t="s">
         <v>483</v>
@@ -38430,7 +38430,7 @@
       <c r="F36" s="124"/>
       <c r="G36" s="124"/>
       <c r="H36" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I36" s="123" t="s">
         <v>483</v>
@@ -38462,10 +38462,10 @@
         <v>22</v>
       </c>
       <c r="B37" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C37" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C37" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D37" s="123" t="s">
         <v>484</v>
@@ -38474,7 +38474,7 @@
       <c r="F37" s="124"/>
       <c r="G37" s="124"/>
       <c r="H37" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I37" s="123" t="s">
         <v>484</v>
@@ -38506,10 +38506,10 @@
         <v>22</v>
       </c>
       <c r="B38" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C38" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C38" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D38" s="123" t="s">
         <v>485</v>
@@ -38518,7 +38518,7 @@
       <c r="F38" s="124"/>
       <c r="G38" s="124"/>
       <c r="H38" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I38" s="123" t="s">
         <v>485</v>
@@ -38550,10 +38550,10 @@
         <v>22</v>
       </c>
       <c r="B39" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C39" s="124" t="s">
         <v>557</v>
-      </c>
-      <c r="C39" s="124" t="s">
-        <v>558</v>
       </c>
       <c r="D39" s="123" t="s">
         <v>486</v>
@@ -38562,7 +38562,7 @@
       <c r="F39" s="124"/>
       <c r="G39" s="124"/>
       <c r="H39" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I39" s="123" t="s">
         <v>486</v>
@@ -38594,22 +38594,22 @@
         <v>22</v>
       </c>
       <c r="B40" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C40" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C40" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D40" s="123" t="s">
-        <v>487</v>
+        <v>569</v>
       </c>
       <c r="E40" s="124"/>
       <c r="F40" s="124"/>
       <c r="G40" s="124"/>
       <c r="H40" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I40" s="123" t="s">
-        <v>487</v>
+        <v>569</v>
       </c>
       <c r="J40" s="123" t="s">
         <v>110</v>
@@ -38638,22 +38638,22 @@
         <v>22</v>
       </c>
       <c r="B41" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C41" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C41" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D41" s="123" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E41" s="124"/>
       <c r="F41" s="124"/>
       <c r="G41" s="124"/>
       <c r="H41" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I41" s="123" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J41" s="123" t="s">
         <v>110</v>
@@ -38682,22 +38682,22 @@
         <v>22</v>
       </c>
       <c r="B42" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C42" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C42" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D42" s="123" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E42" s="124"/>
       <c r="F42" s="124"/>
       <c r="G42" s="124"/>
       <c r="H42" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I42" s="123" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J42" s="123" t="s">
         <v>110</v>
@@ -38726,22 +38726,22 @@
         <v>22</v>
       </c>
       <c r="B43" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C43" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C43" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D43" s="123" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E43" s="124"/>
       <c r="F43" s="124"/>
       <c r="G43" s="124"/>
       <c r="H43" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I43" s="123" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J43" s="123" t="s">
         <v>109</v>
@@ -38770,24 +38770,24 @@
         <v>22</v>
       </c>
       <c r="B44" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C44" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C44" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D44" s="123" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E44" s="192" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F44" s="124"/>
       <c r="G44" s="124"/>
       <c r="H44" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I44" s="123" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J44" s="123" t="s">
         <v>65</v>
@@ -38802,7 +38802,7 @@
         <v>32</v>
       </c>
       <c r="N44" s="192" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="O44" s="124"/>
       <c r="P44" s="126"/>
@@ -38818,24 +38818,24 @@
         <v>22</v>
       </c>
       <c r="B45" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C45" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C45" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D45" s="123" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E45" s="192" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F45" s="124"/>
       <c r="G45" s="124"/>
       <c r="H45" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I45" s="123" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J45" s="123" t="s">
         <v>65</v>
@@ -38850,7 +38850,7 @@
         <v>32</v>
       </c>
       <c r="N45" s="192" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="O45" s="124"/>
       <c r="P45" s="126"/>
@@ -38866,22 +38866,22 @@
         <v>22</v>
       </c>
       <c r="B46" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C46" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C46" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D46" s="123" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E46" s="124"/>
       <c r="F46" s="124"/>
       <c r="G46" s="124"/>
       <c r="H46" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I46" s="123" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J46" s="123" t="s">
         <v>284</v>
@@ -38910,22 +38910,22 @@
         <v>22</v>
       </c>
       <c r="B47" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C47" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C47" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D47" s="123" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E47" s="124"/>
       <c r="F47" s="124"/>
       <c r="G47" s="124"/>
       <c r="H47" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I47" s="123" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J47" s="123" t="s">
         <v>109</v>
@@ -38940,7 +38940,7 @@
         <v>32</v>
       </c>
       <c r="N47" s="124" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="O47" s="124"/>
       <c r="P47" s="126"/>
@@ -38958,22 +38958,22 @@
         <v>22</v>
       </c>
       <c r="B48" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C48" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C48" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D48" s="123" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E48" s="124"/>
       <c r="F48" s="124"/>
       <c r="G48" s="124"/>
       <c r="H48" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I48" s="123" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J48" s="123" t="s">
         <v>64</v>
@@ -39002,22 +39002,22 @@
         <v>22</v>
       </c>
       <c r="B49" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C49" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C49" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D49" s="123" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E49" s="124"/>
       <c r="F49" s="124"/>
       <c r="G49" s="124"/>
       <c r="H49" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I49" s="123" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J49" s="123" t="s">
         <v>110</v>
@@ -39046,28 +39046,28 @@
         <v>22</v>
       </c>
       <c r="B50" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C50" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C50" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D50" s="123" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E50" s="124"/>
       <c r="F50" s="124"/>
       <c r="G50" s="124"/>
       <c r="H50" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I50" s="123" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="J50" s="123" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K50" s="123" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L50" s="172" t="s">
         <v>59</v>
@@ -39090,22 +39090,22 @@
         <v>22</v>
       </c>
       <c r="B51" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C51" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C51" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D51" s="123" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E51" s="124"/>
       <c r="F51" s="124"/>
       <c r="G51" s="124"/>
       <c r="H51" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I51" s="123" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J51" s="123" t="s">
         <v>276</v>
@@ -39134,22 +39134,22 @@
         <v>22</v>
       </c>
       <c r="B52" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C52" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C52" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D52" s="123" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E52" s="124"/>
       <c r="F52" s="124"/>
       <c r="G52" s="124"/>
       <c r="H52" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I52" s="123" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J52" s="123" t="s">
         <v>112</v>
@@ -39178,22 +39178,22 @@
         <v>22</v>
       </c>
       <c r="B53" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C53" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C53" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D53" s="123" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E53" s="124"/>
       <c r="F53" s="124"/>
       <c r="G53" s="124"/>
       <c r="H53" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I53" s="123" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J53" s="123" t="s">
         <v>284</v>
@@ -39222,22 +39222,22 @@
         <v>22</v>
       </c>
       <c r="B54" s="196" t="s">
+        <v>556</v>
+      </c>
+      <c r="C54" s="124" t="s">
         <v>557</v>
       </c>
-      <c r="C54" s="124" t="s">
-        <v>558</v>
-      </c>
       <c r="D54" s="123" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E54" s="124"/>
       <c r="F54" s="124"/>
       <c r="G54" s="124"/>
       <c r="H54" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I54" s="123" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J54" s="123" t="s">
         <v>284</v>
@@ -39272,7 +39272,7 @@
       <c r="F55" s="124"/>
       <c r="G55" s="124"/>
       <c r="H55" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I55" s="124" t="s">
         <v>51</v>
@@ -39310,7 +39310,7 @@
       <c r="F56" s="124"/>
       <c r="G56" s="124"/>
       <c r="H56" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I56" s="124" t="s">
         <v>52</v>
@@ -39348,7 +39348,7 @@
       <c r="F57" s="124"/>
       <c r="G57" s="124"/>
       <c r="H57" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I57" s="124" t="s">
         <v>53</v>
@@ -39386,7 +39386,7 @@
       <c r="F58" s="124"/>
       <c r="G58" s="124"/>
       <c r="H58" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I58" s="124" t="s">
         <v>54</v>
@@ -39426,7 +39426,7 @@
       <c r="F59" s="124"/>
       <c r="G59" s="124"/>
       <c r="H59" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I59" s="124" t="s">
         <v>55</v>
@@ -39462,7 +39462,7 @@
       <c r="F60" s="122"/>
       <c r="G60" s="122"/>
       <c r="H60" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I60" s="124" t="s">
         <v>56</v>
@@ -39613,7 +39613,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="163" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C2" s="163" t="s">
         <v>423</v>
@@ -39627,7 +39627,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="165" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I2" s="162"/>
       <c r="J2" s="162"/>
@@ -39673,13 +39673,13 @@
       <c r="F3" s="124"/>
       <c r="G3" s="124"/>
       <c r="H3" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I3" s="171" t="s">
         <v>418</v>
       </c>
       <c r="J3" s="171" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K3" s="123"/>
       <c r="L3" s="171" t="s">
@@ -39689,7 +39689,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="124" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="O3" s="124"/>
       <c r="P3" s="126"/>
@@ -39707,7 +39707,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="179" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C4" s="124" t="s">
         <v>423</v>
@@ -39718,7 +39718,7 @@
       <c r="F4" s="124"/>
       <c r="G4" s="124"/>
       <c r="H4" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I4" s="123" t="s">
         <v>419</v>
@@ -39749,7 +39749,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="179" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C5" s="124" t="s">
         <v>423</v>
@@ -39761,7 +39761,7 @@
       <c r="F5" s="124"/>
       <c r="G5" s="124"/>
       <c r="H5" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I5" s="123" t="s">
         <v>420</v>
@@ -39797,13 +39797,13 @@
         <v>22</v>
       </c>
       <c r="B6" s="179" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C6" s="124" t="s">
         <v>423</v>
       </c>
       <c r="D6" s="123" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E6" s="124" t="s">
         <v>425</v>
@@ -39811,10 +39811,10 @@
       <c r="F6" s="124"/>
       <c r="G6" s="124"/>
       <c r="H6" s="124" t="s">
+        <v>512</v>
+      </c>
+      <c r="I6" s="123" t="s">
         <v>513</v>
-      </c>
-      <c r="I6" s="123" t="s">
-        <v>514</v>
       </c>
       <c r="J6" s="123" t="s">
         <v>65</v>
@@ -39845,22 +39845,22 @@
         <v>22</v>
       </c>
       <c r="B7" s="179" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C7" s="124" t="s">
         <v>423</v>
       </c>
       <c r="D7" s="123" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E7" s="124"/>
       <c r="F7" s="124"/>
       <c r="G7" s="124"/>
       <c r="H7" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I7" s="123" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J7" s="123" t="s">
         <v>426</v>
@@ -39889,22 +39889,22 @@
         <v>22</v>
       </c>
       <c r="B8" s="179" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C8" s="124" t="s">
         <v>423</v>
       </c>
       <c r="D8" s="123" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E8" s="124"/>
       <c r="F8" s="124"/>
       <c r="G8" s="124"/>
       <c r="H8" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I8" s="123" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J8" s="123" t="s">
         <v>426</v>
@@ -39939,7 +39939,7 @@
       <c r="F9" s="124"/>
       <c r="G9" s="124"/>
       <c r="H9" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I9" s="124" t="s">
         <v>51</v>
@@ -39977,7 +39977,7 @@
       <c r="F10" s="124"/>
       <c r="G10" s="124"/>
       <c r="H10" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I10" s="124" t="s">
         <v>52</v>
@@ -40015,7 +40015,7 @@
       <c r="F11" s="124"/>
       <c r="G11" s="124"/>
       <c r="H11" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I11" s="124" t="s">
         <v>53</v>
@@ -40053,7 +40053,7 @@
       <c r="F12" s="124"/>
       <c r="G12" s="124"/>
       <c r="H12" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I12" s="124" t="s">
         <v>54</v>
@@ -40093,7 +40093,7 @@
       <c r="F13" s="124"/>
       <c r="G13" s="124"/>
       <c r="H13" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I13" s="124" t="s">
         <v>55</v>
@@ -40129,7 +40129,7 @@
       <c r="F14" s="122"/>
       <c r="G14" s="122"/>
       <c r="H14" s="124" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I14" s="124" t="s">
         <v>56</v>
@@ -40294,7 +40294,7 @@
         <v>431</v>
       </c>
       <c r="H2" s="181" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I2" s="168"/>
       <c r="J2" s="168"/>
@@ -40322,7 +40322,7 @@
         <v>N</v>
       </c>
       <c r="T2" s="168" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="U2" s="181" t="s">
         <v>390</v>
@@ -40348,7 +40348,7 @@
       <c r="F3" s="124"/>
       <c r="G3" s="124"/>
       <c r="H3" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I3" s="123" t="s">
         <v>432</v>
@@ -40386,16 +40386,16 @@
         <v>430</v>
       </c>
       <c r="D4" s="123" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E4" s="124"/>
       <c r="F4" s="124"/>
       <c r="G4" s="124"/>
       <c r="H4" s="124" t="s">
+        <v>516</v>
+      </c>
+      <c r="I4" s="123" t="s">
         <v>517</v>
-      </c>
-      <c r="I4" s="123" t="s">
-        <v>518</v>
       </c>
       <c r="J4" s="123" t="s">
         <v>64</v>
@@ -40410,7 +40410,7 @@
         <v>32</v>
       </c>
       <c r="N4" s="124" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="O4" s="125"/>
       <c r="P4" s="124"/>
@@ -40434,16 +40434,16 @@
         <v>430</v>
       </c>
       <c r="D5" s="123" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E5" s="124"/>
       <c r="F5" s="124"/>
       <c r="G5" s="124"/>
       <c r="H5" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I5" s="123" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J5" s="123" t="s">
         <v>64</v>
@@ -40484,7 +40484,7 @@
       <c r="F6" s="124"/>
       <c r="G6" s="124"/>
       <c r="H6" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I6" s="123" t="s">
         <v>437</v>
@@ -40522,7 +40522,7 @@
         <v>430</v>
       </c>
       <c r="D7" s="123" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E7" s="124" t="s">
         <v>438</v>
@@ -40530,10 +40530,10 @@
       <c r="F7" s="124"/>
       <c r="G7" s="124"/>
       <c r="H7" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I7" s="123" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J7" s="123" t="s">
         <v>114</v>
@@ -40570,7 +40570,7 @@
         <v>430</v>
       </c>
       <c r="D8" s="123" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E8" s="124" t="s">
         <v>440</v>
@@ -40578,16 +40578,16 @@
       <c r="F8" s="124"/>
       <c r="G8" s="124"/>
       <c r="H8" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I8" s="123" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J8" s="123" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K8" s="123" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="L8" s="123" t="s">
         <v>59</v>
@@ -40622,7 +40622,7 @@
       <c r="F9" s="124"/>
       <c r="G9" s="124"/>
       <c r="H9" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I9" s="123" t="s">
         <v>441</v>
@@ -40660,16 +40660,16 @@
         <v>430</v>
       </c>
       <c r="D10" s="123" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E10" s="124"/>
       <c r="F10" s="124"/>
       <c r="G10" s="124"/>
       <c r="H10" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I10" s="123" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J10" s="123" t="s">
         <v>449</v>
@@ -40704,16 +40704,16 @@
         <v>430</v>
       </c>
       <c r="D11" s="123" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E11" s="124"/>
       <c r="F11" s="124"/>
       <c r="G11" s="124"/>
       <c r="H11" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I11" s="123" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J11" s="123" t="s">
         <v>449</v>
@@ -40754,7 +40754,7 @@
       <c r="F12" s="124"/>
       <c r="G12" s="124"/>
       <c r="H12" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I12" s="123" t="s">
         <v>433</v>
@@ -40802,7 +40802,7 @@
       <c r="F13" s="124"/>
       <c r="G13" s="124"/>
       <c r="H13" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I13" s="123" t="s">
         <v>435</v>
@@ -40844,16 +40844,16 @@
         <v>430</v>
       </c>
       <c r="D14" s="123" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E14" s="123"/>
       <c r="F14" s="124"/>
       <c r="G14" s="124"/>
       <c r="H14" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I14" s="123" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J14" s="123" t="s">
         <v>110</v>
@@ -40888,16 +40888,16 @@
         <v>430</v>
       </c>
       <c r="D15" s="123" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E15" s="123"/>
       <c r="F15" s="124"/>
       <c r="G15" s="124"/>
       <c r="H15" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I15" s="123" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J15" s="123" t="s">
         <v>110</v>
@@ -40932,16 +40932,16 @@
         <v>430</v>
       </c>
       <c r="D16" s="123" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E16" s="124"/>
       <c r="F16" s="124"/>
       <c r="G16" s="124"/>
       <c r="H16" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I16" s="123" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J16" s="123" t="s">
         <v>61</v>
@@ -40976,16 +40976,16 @@
         <v>430</v>
       </c>
       <c r="D17" s="123" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E17" s="124"/>
       <c r="F17" s="124"/>
       <c r="G17" s="124"/>
       <c r="H17" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I17" s="123" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J17" s="123" t="s">
         <v>61</v>
@@ -41026,7 +41026,7 @@
       <c r="F18" s="124"/>
       <c r="G18" s="124"/>
       <c r="H18" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I18" s="123" t="s">
         <v>442</v>
@@ -41064,16 +41064,16 @@
         <v>430</v>
       </c>
       <c r="D19" s="123" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E19" s="124"/>
       <c r="F19" s="124"/>
       <c r="G19" s="124"/>
       <c r="H19" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I19" s="123" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="J19" s="123" t="s">
         <v>115</v>
@@ -41114,7 +41114,7 @@
       <c r="F20" s="124"/>
       <c r="G20" s="124"/>
       <c r="H20" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I20" s="123" t="s">
         <v>443</v>
@@ -41152,16 +41152,16 @@
         <v>430</v>
       </c>
       <c r="D21" s="123" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E21" s="124"/>
       <c r="F21" s="124"/>
       <c r="G21" s="124"/>
       <c r="H21" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I21" s="123" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J21" s="123" t="s">
         <v>110</v>
@@ -41202,7 +41202,7 @@
       <c r="F22" s="124"/>
       <c r="G22" s="124"/>
       <c r="H22" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I22" s="123" t="s">
         <v>444</v>
@@ -41240,7 +41240,7 @@
       <c r="F23" s="124"/>
       <c r="G23" s="124"/>
       <c r="H23" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I23" s="124" t="s">
         <v>51</v>
@@ -41278,7 +41278,7 @@
       <c r="F24" s="124"/>
       <c r="G24" s="124"/>
       <c r="H24" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I24" s="124" t="s">
         <v>52</v>
@@ -41316,7 +41316,7 @@
       <c r="F25" s="124"/>
       <c r="G25" s="124"/>
       <c r="H25" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I25" s="124" t="s">
         <v>53</v>
@@ -41354,7 +41354,7 @@
       <c r="F26" s="124"/>
       <c r="G26" s="124"/>
       <c r="H26" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I26" s="124" t="s">
         <v>54</v>
@@ -41392,7 +41392,7 @@
       <c r="F27" s="124"/>
       <c r="G27" s="124"/>
       <c r="H27" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I27" s="124" t="s">
         <v>55</v>
@@ -41428,7 +41428,7 @@
       <c r="F28" s="122"/>
       <c r="G28" s="122"/>
       <c r="H28" s="124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I28" s="124" t="s">
         <v>56</v>
@@ -41577,7 +41577,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="186" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C2" s="166" t="s">
         <v>259</v>
@@ -41591,7 +41591,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="203" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I2" s="166"/>
       <c r="J2" s="166"/>
@@ -41632,22 +41632,22 @@
         <v>22</v>
       </c>
       <c r="B3" s="197" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C3" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D3" s="123" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E3" s="124"/>
       <c r="F3" s="124"/>
       <c r="G3" s="124"/>
       <c r="H3" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I3" s="123" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J3" s="123" t="s">
         <v>450</v>
@@ -41662,7 +41662,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="124" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="O3" s="124"/>
       <c r="P3" s="126"/>
@@ -41680,22 +41680,22 @@
         <v>22</v>
       </c>
       <c r="B4" s="197" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C4" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D4" s="123" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E4" s="124"/>
       <c r="F4" s="124"/>
       <c r="G4" s="124"/>
       <c r="H4" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I4" s="123" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J4" s="123" t="s">
         <v>447</v>
@@ -41724,22 +41724,22 @@
         <v>22</v>
       </c>
       <c r="B5" s="197" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C5" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D5" s="123" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E5" s="124"/>
       <c r="F5" s="124"/>
       <c r="G5" s="124"/>
       <c r="H5" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I5" s="123" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J5" s="123" t="s">
         <v>448</v>
@@ -41768,22 +41768,22 @@
         <v>22</v>
       </c>
       <c r="B6" s="197" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C6" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D6" s="123" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E6" s="124"/>
       <c r="F6" s="124"/>
       <c r="G6" s="124"/>
       <c r="H6" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I6" s="123" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J6" s="123" t="s">
         <v>62</v>
@@ -41812,22 +41812,22 @@
         <v>22</v>
       </c>
       <c r="B7" s="197" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C7" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D7" s="123" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E7" s="124"/>
       <c r="F7" s="124"/>
       <c r="G7" s="124"/>
       <c r="H7" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I7" s="123" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J7" s="123" t="s">
         <v>279</v>
@@ -41856,22 +41856,22 @@
         <v>22</v>
       </c>
       <c r="B8" s="197" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C8" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D8" s="123" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E8" s="124"/>
       <c r="F8" s="124"/>
       <c r="G8" s="124"/>
       <c r="H8" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I8" s="123" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J8" s="123" t="s">
         <v>422</v>
@@ -41900,24 +41900,24 @@
         <v>22</v>
       </c>
       <c r="B9" s="197" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C9" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D9" s="123" t="s">
+        <v>539</v>
+      </c>
+      <c r="E9" s="124" t="s">
         <v>540</v>
-      </c>
-      <c r="E9" s="124" t="s">
-        <v>541</v>
       </c>
       <c r="F9" s="124"/>
       <c r="G9" s="124"/>
       <c r="H9" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I9" s="123" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J9" s="123" t="s">
         <v>65</v>
@@ -41932,7 +41932,7 @@
         <v>32</v>
       </c>
       <c r="N9" s="124" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="O9" s="124"/>
       <c r="P9" s="126"/>
@@ -41954,7 +41954,7 @@
       <c r="F10" s="124"/>
       <c r="G10" s="124"/>
       <c r="H10" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I10" s="124" t="s">
         <v>51</v>
@@ -41992,7 +41992,7 @@
       <c r="F11" s="124"/>
       <c r="G11" s="124"/>
       <c r="H11" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I11" s="124" t="s">
         <v>52</v>
@@ -42030,7 +42030,7 @@
       <c r="F12" s="124"/>
       <c r="G12" s="124"/>
       <c r="H12" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I12" s="124" t="s">
         <v>53</v>
@@ -42068,7 +42068,7 @@
       <c r="F13" s="124"/>
       <c r="G13" s="124"/>
       <c r="H13" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I13" s="124" t="s">
         <v>54</v>
@@ -42108,7 +42108,7 @@
       <c r="F14" s="124"/>
       <c r="G14" s="124"/>
       <c r="H14" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I14" s="124" t="s">
         <v>55</v>
@@ -42144,7 +42144,7 @@
       <c r="F15" s="122"/>
       <c r="G15" s="122"/>
       <c r="H15" s="170" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I15" s="124" t="s">
         <v>56</v>
@@ -42192,21 +42192,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C723A6D629A244B9035064CEA29699F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="439c1f6a0871fabbc20469cf751fc22a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c6a5f84-dc80-404b-9608-a58c80d813cf" xmlns:ns3="fb15ab9c-5ce3-4966-97a0-841ffe55082a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a0ba7a63f3f3ddebd5188756dbc3799" ns2:_="" ns3:_="">
     <xsd:import namespace="5c6a5f84-dc80-404b-9608-a58c80d813cf"/>
@@ -42423,24 +42408,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86484D21-336C-4699-B297-37FD20E87A03}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6CC5F60-7C71-49F9-855C-F002D6759E81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D51A253-8FCC-480C-8849-892D45D1BD92}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42457,4 +42440,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6CC5F60-7C71-49F9-855C-F002D6759E81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86484D21-336C-4699-B297-37FD20E87A03}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
RE: STM update V1.0 - Final Review Phase 1 Combined Feeds
Modified the Encryption columns as per DTAC revision as well as column data type got change as well for certain feed
</commit_message>
<xml_diff>
--- a/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.1.xlsx
+++ b/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telenor-AEP\Requirement-Docs\DTAC_Sprint1_SS_Feeds\IS_DTAC_Feeds\Review_Feb2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telenor-AEP\Requirement-Docs\DTAC_STM_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Document - Sign-off" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4049" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4051" uniqueCount="571">
   <si>
     <t>Mode of Integration</t>
   </si>
@@ -1774,6 +1774,9 @@
   </si>
   <si>
     <t>COMP_CODE</t>
+  </si>
+  <si>
+    <t>encrypt(EMAIL_ID)</t>
   </si>
 </sst>
 </file>
@@ -4651,9 +4654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q100" sqref="Q100"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I44" sqref="I44:J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -6219,7 +6222,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="36" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A36" s="24" t="s">
         <v>22</v>
       </c>
@@ -6263,7 +6266,7 @@
       <c r="U36" s="24"/>
       <c r="V36" s="51"/>
     </row>
-    <row r="37" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="37" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A37" s="24" t="s">
         <v>22</v>
       </c>
@@ -6307,7 +6310,7 @@
       <c r="U37" s="24"/>
       <c r="V37" s="51"/>
     </row>
-    <row r="38" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="38" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A38" s="24" t="s">
         <v>22</v>
       </c>
@@ -6351,7 +6354,7 @@
       <c r="U38" s="24"/>
       <c r="V38" s="51"/>
     </row>
-    <row r="39" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="39" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A39" s="24" t="s">
         <v>22</v>
       </c>
@@ -6397,7 +6400,7 @@
       <c r="U39" s="24"/>
       <c r="V39" s="51"/>
     </row>
-    <row r="40" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="40" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A40" s="24" t="s">
         <v>22</v>
       </c>
@@ -6441,7 +6444,7 @@
       <c r="U40" s="24"/>
       <c r="V40" s="51"/>
     </row>
-    <row r="41" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="41" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A41" s="24" t="s">
         <v>22</v>
       </c>
@@ -6485,7 +6488,7 @@
       <c r="U41" s="24"/>
       <c r="V41" s="51"/>
     </row>
-    <row r="42" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="42" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A42" s="24" t="s">
         <v>22</v>
       </c>
@@ -6529,7 +6532,7 @@
       <c r="U42" s="24"/>
       <c r="V42" s="51"/>
     </row>
-    <row r="43" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="43" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A43" s="24" t="s">
         <v>22</v>
       </c>
@@ -6573,7 +6576,7 @@
       <c r="U43" s="24"/>
       <c r="V43" s="51"/>
     </row>
-    <row r="44" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="44" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A44" s="24" t="s">
         <v>22</v>
       </c>
@@ -6596,7 +6599,7 @@
         <v>84</v>
       </c>
       <c r="J44" s="37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K44" s="37" t="s">
         <v>111</v>
@@ -6607,17 +6610,21 @@
       <c r="M44" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="N44" s="24"/>
+      <c r="N44" s="24" t="s">
+        <v>570</v>
+      </c>
       <c r="O44" s="24"/>
       <c r="P44" s="204"/>
       <c r="Q44" s="24"/>
-      <c r="R44" s="204"/>
+      <c r="R44" s="204" t="s">
+        <v>32</v>
+      </c>
       <c r="S44" s="24"/>
       <c r="T44" s="24"/>
       <c r="U44" s="24"/>
       <c r="V44" s="51"/>
     </row>
-    <row r="45" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="45" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A45" s="24" t="s">
         <v>22</v>
       </c>
@@ -6661,7 +6668,7 @@
       <c r="U45" s="24"/>
       <c r="V45" s="51"/>
     </row>
-    <row r="46" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="46" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A46" s="24" t="s">
         <v>22</v>
       </c>
@@ -6705,7 +6712,7 @@
       <c r="U46" s="24"/>
       <c r="V46" s="51"/>
     </row>
-    <row r="47" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="47" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A47" s="24" t="s">
         <v>22</v>
       </c>
@@ -6749,7 +6756,7 @@
       <c r="U47" s="24"/>
       <c r="V47" s="51"/>
     </row>
-    <row r="48" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="48" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A48" s="24" t="s">
         <v>22</v>
       </c>
@@ -6793,7 +6800,7 @@
       <c r="U48" s="24"/>
       <c r="V48" s="51"/>
     </row>
-    <row r="49" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="49" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A49" s="24" t="s">
         <v>22</v>
       </c>
@@ -6837,7 +6844,7 @@
       <c r="U49" s="24"/>
       <c r="V49" s="51"/>
     </row>
-    <row r="50" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="50" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A50" s="24" t="s">
         <v>22</v>
       </c>
@@ -6881,7 +6888,7 @@
       <c r="U50" s="24"/>
       <c r="V50" s="51"/>
     </row>
-    <row r="51" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="51" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A51" s="24" t="s">
         <v>22</v>
       </c>
@@ -6925,7 +6932,7 @@
       <c r="U51" s="24"/>
       <c r="V51" s="51"/>
     </row>
-    <row r="52" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="52" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A52" s="24" t="s">
         <v>22</v>
       </c>
@@ -6969,7 +6976,7 @@
       <c r="U52" s="24"/>
       <c r="V52" s="51"/>
     </row>
-    <row r="53" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="53" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A53" s="24" t="s">
         <v>22</v>
       </c>
@@ -7013,7 +7020,7 @@
       <c r="U53" s="24"/>
       <c r="V53" s="51"/>
     </row>
-    <row r="54" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="54" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A54" s="24" t="s">
         <v>22</v>
       </c>
@@ -7057,7 +7064,7 @@
       <c r="U54" s="24"/>
       <c r="V54" s="51"/>
     </row>
-    <row r="55" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="55" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A55" s="24" t="s">
         <v>22</v>
       </c>
@@ -7101,7 +7108,7 @@
       <c r="U55" s="24"/>
       <c r="V55" s="51"/>
     </row>
-    <row r="56" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="56" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A56" s="24" t="s">
         <v>22</v>
       </c>
@@ -7149,7 +7156,7 @@
       <c r="U56" s="24"/>
       <c r="V56" s="51"/>
     </row>
-    <row r="57" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="57" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A57" s="24" t="s">
         <v>22</v>
       </c>
@@ -7197,7 +7204,7 @@
       <c r="U57" s="24"/>
       <c r="V57" s="51"/>
     </row>
-    <row r="58" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="58" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A58" s="24" t="s">
         <v>22</v>
       </c>
@@ -7245,7 +7252,7 @@
       <c r="U58" s="24"/>
       <c r="V58" s="51"/>
     </row>
-    <row r="59" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="59" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A59" s="24" t="s">
         <v>22</v>
       </c>
@@ -7293,7 +7300,7 @@
       <c r="U59" s="24"/>
       <c r="V59" s="51"/>
     </row>
-    <row r="60" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="60" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A60" s="24" t="s">
         <v>22</v>
       </c>
@@ -7341,7 +7348,7 @@
       <c r="U60" s="24"/>
       <c r="V60" s="51"/>
     </row>
-    <row r="61" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="61" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A61" s="24" t="s">
         <v>22</v>
       </c>
@@ -7385,7 +7392,7 @@
       <c r="U61" s="24"/>
       <c r="V61" s="51"/>
     </row>
-    <row r="62" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="62" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A62" s="24" t="s">
         <v>22</v>
       </c>
@@ -7429,7 +7436,7 @@
       <c r="U62" s="24"/>
       <c r="V62" s="51"/>
     </row>
-    <row r="63" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="63" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A63" s="24" t="s">
         <v>22</v>
       </c>
@@ -7473,7 +7480,7 @@
       <c r="U63" s="24"/>
       <c r="V63" s="51"/>
     </row>
-    <row r="64" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="64" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A64" s="24" t="s">
         <v>22</v>
       </c>
@@ -7517,7 +7524,7 @@
       <c r="U64" s="24"/>
       <c r="V64" s="51"/>
     </row>
-    <row r="65" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="65" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A65" s="24" t="s">
         <v>22</v>
       </c>
@@ -7565,7 +7572,7 @@
       <c r="U65" s="24"/>
       <c r="V65" s="51"/>
     </row>
-    <row r="66" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="66" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A66" s="24" t="s">
         <v>22</v>
       </c>
@@ -7609,7 +7616,7 @@
       <c r="U66" s="24"/>
       <c r="V66" s="51"/>
     </row>
-    <row r="67" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="67" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A67" s="24" t="s">
         <v>22</v>
       </c>
@@ -7657,7 +7664,7 @@
       <c r="U67" s="24"/>
       <c r="V67" s="51"/>
     </row>
-    <row r="68" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="68" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A68" s="24" t="s">
         <v>22</v>
       </c>
@@ -7705,7 +7712,7 @@
       <c r="U68" s="24"/>
       <c r="V68" s="51"/>
     </row>
-    <row r="69" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="69" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A69" s="24" t="s">
         <v>22</v>
       </c>
@@ -7753,7 +7760,7 @@
       <c r="U69" s="24"/>
       <c r="V69" s="51"/>
     </row>
-    <row r="70" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="70" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A70" s="24" t="s">
         <v>22</v>
       </c>
@@ -7797,7 +7804,7 @@
       <c r="U70" s="24"/>
       <c r="V70" s="51"/>
     </row>
-    <row r="71" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="71" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A71" s="24" t="s">
         <v>22</v>
       </c>
@@ -7841,7 +7848,7 @@
       <c r="U71" s="24"/>
       <c r="V71" s="51"/>
     </row>
-    <row r="72" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="72" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A72" s="24" t="s">
         <v>22</v>
       </c>
@@ -7889,7 +7896,7 @@
       <c r="U72" s="24"/>
       <c r="V72" s="51"/>
     </row>
-    <row r="73" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="73" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A73" s="24" t="s">
         <v>22</v>
       </c>
@@ -7933,7 +7940,7 @@
       <c r="U73" s="24"/>
       <c r="V73" s="51"/>
     </row>
-    <row r="74" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="74" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A74" s="24" t="s">
         <v>22</v>
       </c>
@@ -7977,7 +7984,7 @@
       <c r="U74" s="24"/>
       <c r="V74" s="51"/>
     </row>
-    <row r="75" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="75" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A75" s="24" t="s">
         <v>22</v>
       </c>
@@ -8021,7 +8028,7 @@
       <c r="U75" s="24"/>
       <c r="V75" s="51"/>
     </row>
-    <row r="76" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="76" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A76" s="24"/>
       <c r="B76" s="24"/>
       <c r="C76" s="24"/>
@@ -8059,7 +8066,7 @@
       <c r="U76" s="24"/>
       <c r="V76" s="51"/>
     </row>
-    <row r="77" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="77" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A77" s="24"/>
       <c r="B77" s="24"/>
       <c r="C77" s="24"/>
@@ -8097,7 +8104,7 @@
       <c r="U77" s="24"/>
       <c r="V77" s="51"/>
     </row>
-    <row r="78" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="78" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A78" s="24"/>
       <c r="B78" s="24"/>
       <c r="C78" s="24"/>
@@ -8135,7 +8142,7 @@
       <c r="U78" s="24"/>
       <c r="V78" s="51"/>
     </row>
-    <row r="79" spans="1:22" s="39" customFormat="1" hidden="1" outlineLevel="1">
+    <row r="79" spans="1:22" s="39" customFormat="1" outlineLevel="1">
       <c r="A79" s="24"/>
       <c r="B79" s="24"/>
       <c r="C79" s="24"/>
@@ -8175,7 +8182,7 @@
       <c r="U79" s="24"/>
       <c r="V79" s="51"/>
     </row>
-    <row r="80" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="80" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A80" s="24"/>
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
@@ -8213,7 +8220,7 @@
       <c r="U80" s="24"/>
       <c r="V80" s="51"/>
     </row>
-    <row r="81" spans="1:22" s="39" customFormat="1" ht="12.75" hidden="1" outlineLevel="1">
+    <row r="81" spans="1:22" s="39" customFormat="1" ht="12.75" outlineLevel="1">
       <c r="A81" s="24"/>
       <c r="B81" s="24"/>
       <c r="C81" s="24"/>
@@ -8251,7 +8258,7 @@
       <c r="U81" s="24"/>
       <c r="V81" s="51"/>
     </row>
-    <row r="82" spans="1:22" s="6" customFormat="1" collapsed="1">
+    <row r="82" spans="1:22" s="6" customFormat="1">
       <c r="A82" s="17" t="s">
         <v>22</v>
       </c>
@@ -36797,7 +36804,7 @@
   </sheetPr>
   <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
@@ -42192,6 +42199,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C723A6D629A244B9035064CEA29699F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="439c1f6a0871fabbc20469cf751fc22a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c6a5f84-dc80-404b-9608-a58c80d813cf" xmlns:ns3="fb15ab9c-5ce3-4966-97a0-841ffe55082a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a0ba7a63f3f3ddebd5188756dbc3799" ns2:_="" ns3:_="">
     <xsd:import namespace="5c6a5f84-dc80-404b-9608-a58c80d813cf"/>
@@ -42408,7 +42421,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -42417,13 +42430,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86484D21-336C-4699-B297-37FD20E87A03}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D51A253-8FCC-480C-8849-892D45D1BD92}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42442,19 +42458,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6CC5F60-7C71-49F9-855C-F002D6759E81}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86484D21-336C-4699-B297-37FD20E87A03}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
RE: [AEP-dtac] Ph#2 new feeds development plan #Request 8-Jun-20
Data Roaming feed added with 2 derived and 1 source direct column in STM and ISD attached version
</commit_message>
<xml_diff>
--- a/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.1.xlsx
+++ b/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Document - Sign-off" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CMP!$A$1:$U$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DIM!$A$1:$T$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ESRVC!$A$1:$U$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">MD!$A$1:$U$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">MD!$A$1:$U$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">MDD!$A$1:$U$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">OMR!$A$1:$T$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">RBT!$A$1:$T$1</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4051" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4074" uniqueCount="577">
   <si>
     <t>Mode of Integration</t>
   </si>
@@ -1647,9 +1647,6 @@
     <t>PLMN</t>
   </si>
   <si>
-    <t>FILE_NAME</t>
-  </si>
-  <si>
     <t>encrypt(A_NUMB)</t>
   </si>
   <si>
@@ -1729,12 +1726,6 @@
   </si>
   <si>
     <t>DIM_DIM_DEVICE_CAPABILITIES</t>
-  </si>
-  <si>
-    <t>CouponWs_coupappm[1|2]_TX.LOG</t>
-  </si>
-  <si>
-    <t>&lt;YYYYMMDD&gt;</t>
   </si>
   <si>
     <t>Encrypt(HEADERCONTACTNUMBER)</t>
@@ -1777,6 +1768,33 @@
   </si>
   <si>
     <t>encrypt(EMAIL_ID)</t>
+  </si>
+  <si>
+    <t>SOURCE_FILE_NAME</t>
+  </si>
+  <si>
+    <t>CouponWs_coupappm[1|2]_TX.LOG.YYYYMMDD</t>
+  </si>
+  <si>
+    <t>varchar(400)</t>
+  </si>
+  <si>
+    <t>Because this feed type of CDR, DTAC preparing and merging many to one file. Padding original_filename first column.</t>
+  </si>
+  <si>
+    <t>ORIGINAL_FILENAME</t>
+  </si>
+  <si>
+    <t>ENODE_B</t>
+  </si>
+  <si>
+    <t>FILE_NAME</t>
+  </si>
+  <si>
+    <t>VARCHAR2(400)</t>
+  </si>
+  <si>
+    <t>Source file name which was processed</t>
   </si>
 </sst>
 </file>
@@ -2554,7 +2572,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3056,25 +3074,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="35" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="32" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="33" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="34" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="32" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
@@ -3109,6 +3142,18 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="35" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -3451,12 +3496,12 @@
       <c r="A2" s="55"/>
     </row>
     <row r="3" spans="1:6" ht="20.25">
-      <c r="A3" s="214" t="s">
+      <c r="A3" s="219" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="214"/>
-      <c r="C3" s="214"/>
-      <c r="D3" s="214"/>
+      <c r="B3" s="219"/>
+      <c r="C3" s="219"/>
+      <c r="D3" s="219"/>
     </row>
     <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="55"/>
@@ -3480,10 +3525,10 @@
       <c r="F7" s="61"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="215" t="s">
+      <c r="A8" s="220" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="216"/>
+      <c r="B8" s="221"/>
       <c r="C8" s="62" t="s">
         <v>163</v>
       </c>
@@ -3510,7 +3555,7 @@
       <c r="F9" s="64"/>
     </row>
     <row r="10" spans="1:6" ht="15.75">
-      <c r="A10" s="217" t="s">
+      <c r="A10" s="222" t="s">
         <v>169</v>
       </c>
       <c r="B10" s="66" t="s">
@@ -3522,7 +3567,7 @@
       <c r="F10" s="71"/>
     </row>
     <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="218"/>
+      <c r="A11" s="223"/>
       <c r="B11" s="72" t="s">
         <v>171</v>
       </c>
@@ -3552,7 +3597,7 @@
       <c r="F13" s="71"/>
     </row>
     <row r="14" spans="1:6" ht="15.75">
-      <c r="A14" s="219" t="s">
+      <c r="A14" s="224" t="s">
         <v>174</v>
       </c>
       <c r="B14" s="72" t="s">
@@ -3564,7 +3609,7 @@
       <c r="F14" s="76"/>
     </row>
     <row r="15" spans="1:6" ht="15.75">
-      <c r="A15" s="220"/>
+      <c r="A15" s="225"/>
       <c r="B15" s="66" t="s">
         <v>173</v>
       </c>
@@ -3574,7 +3619,7 @@
       <c r="F15" s="79"/>
     </row>
     <row r="16" spans="1:6" ht="15.75">
-      <c r="A16" s="220"/>
+      <c r="A16" s="225"/>
       <c r="B16" s="66" t="s">
         <v>176</v>
       </c>
@@ -3584,7 +3629,7 @@
       <c r="F16" s="79"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickBot="1">
-      <c r="A17" s="221"/>
+      <c r="A17" s="226"/>
       <c r="B17" s="81" t="s">
         <v>177</v>
       </c>
@@ -3621,11 +3666,11 @@
       <c r="C20" s="88" t="s">
         <v>181</v>
       </c>
-      <c r="D20" s="222" t="s">
+      <c r="D20" s="227" t="s">
         <v>182</v>
       </c>
-      <c r="E20" s="223"/>
-      <c r="F20" s="224"/>
+      <c r="E20" s="228"/>
+      <c r="F20" s="229"/>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1">
       <c r="A21" s="89">
@@ -3637,11 +3682,11 @@
       <c r="C21" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="213" t="s">
+      <c r="D21" s="216" t="s">
         <v>184</v>
       </c>
-      <c r="E21" s="211"/>
-      <c r="F21" s="212"/>
+      <c r="E21" s="217"/>
+      <c r="F21" s="218"/>
     </row>
     <row r="22" spans="1:6" ht="36.75" customHeight="1">
       <c r="A22" s="92">
@@ -3653,11 +3698,11 @@
       <c r="C22" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D22" s="208" t="s">
+      <c r="D22" s="231" t="s">
         <v>186</v>
       </c>
-      <c r="E22" s="208"/>
-      <c r="F22" s="209"/>
+      <c r="E22" s="231"/>
+      <c r="F22" s="232"/>
     </row>
     <row r="23" spans="1:6" ht="31.5" customHeight="1">
       <c r="A23" s="92">
@@ -3669,11 +3714,11 @@
       <c r="C23" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D23" s="208" t="s">
+      <c r="D23" s="231" t="s">
         <v>187</v>
       </c>
-      <c r="E23" s="208"/>
-      <c r="F23" s="209"/>
+      <c r="E23" s="231"/>
+      <c r="F23" s="232"/>
     </row>
     <row r="24" spans="1:6" ht="44.25" customHeight="1">
       <c r="A24" s="92">
@@ -3685,11 +3730,11 @@
       <c r="C24" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D24" s="208" t="s">
+      <c r="D24" s="231" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="208"/>
-      <c r="F24" s="209"/>
+      <c r="E24" s="231"/>
+      <c r="F24" s="232"/>
     </row>
     <row r="25" spans="1:6" ht="89.25" customHeight="1">
       <c r="A25" s="92">
@@ -3701,11 +3746,11 @@
       <c r="C25" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D25" s="210" t="s">
+      <c r="D25" s="233" t="s">
         <v>189</v>
       </c>
-      <c r="E25" s="211"/>
-      <c r="F25" s="212"/>
+      <c r="E25" s="217"/>
+      <c r="F25" s="218"/>
     </row>
     <row r="26" spans="1:6" ht="44.25" customHeight="1">
       <c r="A26" s="92">
@@ -3717,11 +3762,11 @@
       <c r="C26" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D26" s="207" t="s">
+      <c r="D26" s="230" t="s">
         <v>190</v>
       </c>
-      <c r="E26" s="207"/>
-      <c r="F26" s="207"/>
+      <c r="E26" s="230"/>
+      <c r="F26" s="230"/>
     </row>
     <row r="27" spans="1:6" ht="44.25" customHeight="1">
       <c r="A27" s="92">
@@ -3733,11 +3778,11 @@
       <c r="C27" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="207" t="s">
+      <c r="D27" s="230" t="s">
         <v>191</v>
       </c>
-      <c r="E27" s="207"/>
-      <c r="F27" s="207"/>
+      <c r="E27" s="230"/>
+      <c r="F27" s="230"/>
     </row>
     <row r="28" spans="1:6" ht="44.25" customHeight="1">
       <c r="A28" s="92" t="s">
@@ -3749,11 +3794,11 @@
       <c r="C28" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="207" t="s">
+      <c r="D28" s="230" t="s">
         <v>193</v>
       </c>
-      <c r="E28" s="207"/>
-      <c r="F28" s="207"/>
+      <c r="E28" s="230"/>
+      <c r="F28" s="230"/>
     </row>
     <row r="29" spans="1:6" ht="54" customHeight="1">
       <c r="A29" s="92">
@@ -3765,20 +3810,14 @@
       <c r="C29" s="94" t="s">
         <v>185</v>
       </c>
-      <c r="D29" s="207" t="s">
-        <v>567</v>
-      </c>
-      <c r="E29" s="207"/>
-      <c r="F29" s="207"/>
+      <c r="D29" s="230" t="s">
+        <v>564</v>
+      </c>
+      <c r="E29" s="230"/>
+      <c r="F29" s="230"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D22:F22"/>
@@ -3787,6 +3826,12 @@
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4654,9 +4699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44:J44"/>
+      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -4757,7 +4802,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>23</v>
@@ -4808,7 +4853,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>23</v>
@@ -4854,7 +4899,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>23</v>
@@ -4898,7 +4943,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>23</v>
@@ -4942,7 +4987,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>23</v>
@@ -4986,7 +5031,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>23</v>
@@ -5030,7 +5075,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>23</v>
@@ -5074,7 +5119,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>23</v>
@@ -5122,7 +5167,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>23</v>
@@ -5166,7 +5211,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>23</v>
@@ -5445,7 +5490,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>23</v>
@@ -5496,7 +5541,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>23</v>
@@ -5542,7 +5587,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>23</v>
@@ -5586,7 +5631,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>23</v>
@@ -5630,7 +5675,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>23</v>
@@ -5674,7 +5719,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>23</v>
@@ -5718,7 +5763,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>23</v>
@@ -5762,7 +5807,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>23</v>
@@ -5806,7 +5851,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>23</v>
@@ -5854,7 +5899,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>23</v>
@@ -5902,7 +5947,7 @@
         <v>22</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>23</v>
@@ -6176,7 +6221,7 @@
         <v>22</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>23</v>
@@ -6227,7 +6272,7 @@
         <v>22</v>
       </c>
       <c r="B36" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C36" s="25" t="s">
         <v>23</v>
@@ -6271,7 +6316,7 @@
         <v>22</v>
       </c>
       <c r="B37" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>23</v>
@@ -6315,7 +6360,7 @@
         <v>22</v>
       </c>
       <c r="B38" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>23</v>
@@ -6359,7 +6404,7 @@
         <v>22</v>
       </c>
       <c r="B39" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C39" s="25" t="s">
         <v>23</v>
@@ -6405,7 +6450,7 @@
         <v>22</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C40" s="25" t="s">
         <v>23</v>
@@ -6449,7 +6494,7 @@
         <v>22</v>
       </c>
       <c r="B41" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C41" s="25" t="s">
         <v>23</v>
@@ -6493,7 +6538,7 @@
         <v>22</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C42" s="25" t="s">
         <v>23</v>
@@ -6537,7 +6582,7 @@
         <v>22</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C43" s="25" t="s">
         <v>23</v>
@@ -6581,7 +6626,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C44" s="25" t="s">
         <v>23</v>
@@ -6611,7 +6656,7 @@
         <v>32</v>
       </c>
       <c r="N44" s="24" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="O44" s="24"/>
       <c r="P44" s="204"/>
@@ -6629,7 +6674,7 @@
         <v>22</v>
       </c>
       <c r="B45" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>23</v>
@@ -6673,7 +6718,7 @@
         <v>22</v>
       </c>
       <c r="B46" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C46" s="25" t="s">
         <v>23</v>
@@ -6717,7 +6762,7 @@
         <v>22</v>
       </c>
       <c r="B47" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C47" s="25" t="s">
         <v>23</v>
@@ -6761,7 +6806,7 @@
         <v>22</v>
       </c>
       <c r="B48" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C48" s="25" t="s">
         <v>23</v>
@@ -6805,7 +6850,7 @@
         <v>22</v>
       </c>
       <c r="B49" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C49" s="25" t="s">
         <v>23</v>
@@ -6849,7 +6894,7 @@
         <v>22</v>
       </c>
       <c r="B50" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>23</v>
@@ -6893,7 +6938,7 @@
         <v>22</v>
       </c>
       <c r="B51" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>23</v>
@@ -6937,7 +6982,7 @@
         <v>22</v>
       </c>
       <c r="B52" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C52" s="25" t="s">
         <v>23</v>
@@ -6981,7 +7026,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C53" s="25" t="s">
         <v>23</v>
@@ -7025,7 +7070,7 @@
         <v>22</v>
       </c>
       <c r="B54" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C54" s="25" t="s">
         <v>23</v>
@@ -7069,7 +7114,7 @@
         <v>22</v>
       </c>
       <c r="B55" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>23</v>
@@ -7113,7 +7158,7 @@
         <v>22</v>
       </c>
       <c r="B56" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>23</v>
@@ -7143,7 +7188,7 @@
         <v>32</v>
       </c>
       <c r="N56" s="24" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="O56" s="24"/>
       <c r="P56" s="204"/>
@@ -7161,7 +7206,7 @@
         <v>22</v>
       </c>
       <c r="B57" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C57" s="25" t="s">
         <v>23</v>
@@ -7191,7 +7236,7 @@
         <v>32</v>
       </c>
       <c r="N57" s="24" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="O57" s="24"/>
       <c r="P57" s="204"/>
@@ -7209,7 +7254,7 @@
         <v>22</v>
       </c>
       <c r="B58" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C58" s="25" t="s">
         <v>23</v>
@@ -7239,7 +7284,7 @@
         <v>32</v>
       </c>
       <c r="N58" s="24" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="O58" s="24"/>
       <c r="P58" s="204"/>
@@ -7257,7 +7302,7 @@
         <v>22</v>
       </c>
       <c r="B59" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>23</v>
@@ -7287,7 +7332,7 @@
         <v>32</v>
       </c>
       <c r="N59" s="24" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="O59" s="24"/>
       <c r="P59" s="204"/>
@@ -7305,7 +7350,7 @@
         <v>22</v>
       </c>
       <c r="B60" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>23</v>
@@ -7335,7 +7380,7 @@
         <v>32</v>
       </c>
       <c r="N60" s="24" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="O60" s="24"/>
       <c r="P60" s="204"/>
@@ -7353,13 +7398,13 @@
         <v>22</v>
       </c>
       <c r="B61" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D61" s="206" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
@@ -7368,7 +7413,7 @@
         <v>27</v>
       </c>
       <c r="I61" s="206" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="J61" s="37" t="s">
         <v>62</v>
@@ -7397,13 +7442,13 @@
         <v>22</v>
       </c>
       <c r="B62" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>23</v>
       </c>
       <c r="D62" s="206" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
@@ -7412,7 +7457,7 @@
         <v>27</v>
       </c>
       <c r="I62" s="206" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J62" s="37" t="s">
         <v>62</v>
@@ -7441,7 +7486,7 @@
         <v>22</v>
       </c>
       <c r="B63" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>23</v>
@@ -7485,7 +7530,7 @@
         <v>22</v>
       </c>
       <c r="B64" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>23</v>
@@ -7529,7 +7574,7 @@
         <v>22</v>
       </c>
       <c r="B65" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C65" s="25" t="s">
         <v>23</v>
@@ -7577,7 +7622,7 @@
         <v>22</v>
       </c>
       <c r="B66" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C66" s="25" t="s">
         <v>23</v>
@@ -7621,7 +7666,7 @@
         <v>22</v>
       </c>
       <c r="B67" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C67" s="25" t="s">
         <v>23</v>
@@ -7669,7 +7714,7 @@
         <v>22</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C68" s="25" t="s">
         <v>23</v>
@@ -7717,7 +7762,7 @@
         <v>22</v>
       </c>
       <c r="B69" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C69" s="25" t="s">
         <v>23</v>
@@ -7765,7 +7810,7 @@
         <v>22</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C70" s="25" t="s">
         <v>23</v>
@@ -7809,7 +7854,7 @@
         <v>22</v>
       </c>
       <c r="B71" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C71" s="25" t="s">
         <v>23</v>
@@ -7853,7 +7898,7 @@
         <v>22</v>
       </c>
       <c r="B72" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C72" s="25" t="s">
         <v>23</v>
@@ -7901,7 +7946,7 @@
         <v>22</v>
       </c>
       <c r="B73" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C73" s="25" t="s">
         <v>23</v>
@@ -7945,7 +7990,7 @@
         <v>22</v>
       </c>
       <c r="B74" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C74" s="25" t="s">
         <v>23</v>
@@ -7989,7 +8034,7 @@
         <v>22</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C75" s="25" t="s">
         <v>23</v>
@@ -8263,7 +8308,7 @@
         <v>22</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C82" s="19" t="s">
         <v>23</v>
@@ -8314,7 +8359,7 @@
         <v>22</v>
       </c>
       <c r="B83" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C83" s="26" t="s">
         <v>23</v>
@@ -8360,7 +8405,7 @@
         <v>22</v>
       </c>
       <c r="B84" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C84" s="26" t="s">
         <v>23</v>
@@ -8404,7 +8449,7 @@
         <v>22</v>
       </c>
       <c r="B85" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C85" s="26" t="s">
         <v>23</v>
@@ -8448,7 +8493,7 @@
         <v>22</v>
       </c>
       <c r="B86" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C86" s="26" t="s">
         <v>23</v>
@@ -8492,7 +8537,7 @@
         <v>22</v>
       </c>
       <c r="B87" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C87" s="26" t="s">
         <v>23</v>
@@ -8536,7 +8581,7 @@
         <v>22</v>
       </c>
       <c r="B88" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C88" s="26" t="s">
         <v>23</v>
@@ -8580,7 +8625,7 @@
         <v>22</v>
       </c>
       <c r="B89" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C89" s="26" t="s">
         <v>23</v>
@@ -8624,7 +8669,7 @@
         <v>22</v>
       </c>
       <c r="B90" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C90" s="26" t="s">
         <v>23</v>
@@ -8672,7 +8717,7 @@
         <v>22</v>
       </c>
       <c r="B91" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C91" s="26" t="s">
         <v>23</v>
@@ -8716,7 +8761,7 @@
         <v>22</v>
       </c>
       <c r="B92" s="48" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C92" s="26" t="s">
         <v>23</v>
@@ -8994,7 +9039,7 @@
         <v>22</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C99" s="9" t="s">
         <v>23</v>
@@ -9045,7 +9090,7 @@
         <v>22</v>
       </c>
       <c r="B100" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C100" s="26" t="s">
         <v>23</v>
@@ -9091,7 +9136,7 @@
         <v>22</v>
       </c>
       <c r="B101" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C101" s="26" t="s">
         <v>23</v>
@@ -9135,7 +9180,7 @@
         <v>22</v>
       </c>
       <c r="B102" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C102" s="26" t="s">
         <v>23</v>
@@ -9179,7 +9224,7 @@
         <v>22</v>
       </c>
       <c r="B103" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C103" s="26" t="s">
         <v>23</v>
@@ -9223,7 +9268,7 @@
         <v>22</v>
       </c>
       <c r="B104" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C104" s="26" t="s">
         <v>23</v>
@@ -9267,7 +9312,7 @@
         <v>22</v>
       </c>
       <c r="B105" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C105" s="26" t="s">
         <v>23</v>
@@ -9311,7 +9356,7 @@
         <v>22</v>
       </c>
       <c r="B106" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C106" s="26" t="s">
         <v>23</v>
@@ -9355,7 +9400,7 @@
         <v>22</v>
       </c>
       <c r="B107" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C107" s="26" t="s">
         <v>23</v>
@@ -9399,7 +9444,7 @@
         <v>22</v>
       </c>
       <c r="B108" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C108" s="26" t="s">
         <v>23</v>
@@ -9443,7 +9488,7 @@
         <v>22</v>
       </c>
       <c r="B109" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C109" s="26" t="s">
         <v>23</v>
@@ -9487,7 +9532,7 @@
         <v>22</v>
       </c>
       <c r="B110" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C110" s="26" t="s">
         <v>23</v>
@@ -9531,7 +9576,7 @@
         <v>22</v>
       </c>
       <c r="B111" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C111" s="26" t="s">
         <v>23</v>
@@ -9575,7 +9620,7 @@
         <v>22</v>
       </c>
       <c r="B112" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C112" s="26" t="s">
         <v>23</v>
@@ -9619,7 +9664,7 @@
         <v>22</v>
       </c>
       <c r="B113" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C113" s="26" t="s">
         <v>23</v>
@@ -9663,7 +9708,7 @@
         <v>22</v>
       </c>
       <c r="B114" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C114" s="26" t="s">
         <v>23</v>
@@ -9707,7 +9752,7 @@
         <v>22</v>
       </c>
       <c r="B115" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C115" s="26" t="s">
         <v>23</v>
@@ -9751,7 +9796,7 @@
         <v>22</v>
       </c>
       <c r="B116" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C116" s="26" t="s">
         <v>23</v>
@@ -9795,7 +9840,7 @@
         <v>22</v>
       </c>
       <c r="B117" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C117" s="26" t="s">
         <v>23</v>
@@ -9839,7 +9884,7 @@
         <v>22</v>
       </c>
       <c r="B118" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C118" s="26" t="s">
         <v>23</v>
@@ -9883,7 +9928,7 @@
         <v>22</v>
       </c>
       <c r="B119" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C119" s="26" t="s">
         <v>23</v>
@@ -9927,7 +9972,7 @@
         <v>22</v>
       </c>
       <c r="B120" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C120" s="26" t="s">
         <v>23</v>
@@ -9971,7 +10016,7 @@
         <v>22</v>
       </c>
       <c r="B121" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C121" s="26" t="s">
         <v>23</v>
@@ -10015,7 +10060,7 @@
         <v>22</v>
       </c>
       <c r="B122" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C122" s="26" t="s">
         <v>23</v>
@@ -10059,7 +10104,7 @@
         <v>22</v>
       </c>
       <c r="B123" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C123" s="26" t="s">
         <v>23</v>
@@ -10103,7 +10148,7 @@
         <v>22</v>
       </c>
       <c r="B124" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C124" s="26" t="s">
         <v>23</v>
@@ -10151,7 +10196,7 @@
         <v>22</v>
       </c>
       <c r="B125" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C125" s="26" t="s">
         <v>23</v>
@@ -10195,7 +10240,7 @@
         <v>22</v>
       </c>
       <c r="B126" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C126" s="26" t="s">
         <v>23</v>
@@ -10239,7 +10284,7 @@
         <v>22</v>
       </c>
       <c r="B127" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C127" s="26" t="s">
         <v>23</v>
@@ -10283,7 +10328,7 @@
         <v>22</v>
       </c>
       <c r="B128" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C128" s="26" t="s">
         <v>23</v>
@@ -10327,7 +10372,7 @@
         <v>22</v>
       </c>
       <c r="B129" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C129" s="26" t="s">
         <v>23</v>
@@ -10375,7 +10420,7 @@
         <v>22</v>
       </c>
       <c r="B130" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C130" s="26" t="s">
         <v>23</v>
@@ -10419,7 +10464,7 @@
         <v>22</v>
       </c>
       <c r="B131" s="48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C131" s="26" t="s">
         <v>23</v>
@@ -10832,7 +10877,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="137" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I2" s="137"/>
       <c r="J2" s="140"/>
@@ -11076,7 +11121,7 @@
       <c r="F3" s="123"/>
       <c r="G3" s="123"/>
       <c r="H3" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I3" s="123" t="s">
         <v>288</v>
@@ -11314,7 +11359,7 @@
       <c r="F4" s="123"/>
       <c r="G4" s="123"/>
       <c r="H4" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I4" s="123" t="s">
         <v>289</v>
@@ -11550,7 +11595,7 @@
       <c r="F5" s="123"/>
       <c r="G5" s="123"/>
       <c r="H5" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I5" s="123" t="s">
         <v>290</v>
@@ -11786,7 +11831,7 @@
       <c r="F6" s="123"/>
       <c r="G6" s="123"/>
       <c r="H6" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I6" s="123" t="s">
         <v>291</v>
@@ -12022,7 +12067,7 @@
       <c r="F7" s="123"/>
       <c r="G7" s="123"/>
       <c r="H7" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I7" s="123" t="s">
         <v>292</v>
@@ -12258,7 +12303,7 @@
       <c r="F8" s="123"/>
       <c r="G8" s="123"/>
       <c r="H8" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I8" s="123" t="s">
         <v>293</v>
@@ -12494,7 +12539,7 @@
       <c r="F9" s="123"/>
       <c r="G9" s="123"/>
       <c r="H9" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I9" s="123" t="s">
         <v>294</v>
@@ -12730,7 +12775,7 @@
       <c r="F10" s="123"/>
       <c r="G10" s="123"/>
       <c r="H10" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I10" s="123" t="s">
         <v>295</v>
@@ -12966,7 +13011,7 @@
       <c r="F11" s="123"/>
       <c r="G11" s="123"/>
       <c r="H11" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I11" s="123" t="s">
         <v>296</v>
@@ -13202,7 +13247,7 @@
       <c r="F12" s="123"/>
       <c r="G12" s="123"/>
       <c r="H12" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I12" s="123" t="s">
         <v>297</v>
@@ -13438,7 +13483,7 @@
       <c r="F13" s="123"/>
       <c r="G13" s="123"/>
       <c r="H13" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I13" s="123" t="s">
         <v>298</v>
@@ -13674,7 +13719,7 @@
       <c r="F14" s="123"/>
       <c r="G14" s="123"/>
       <c r="H14" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I14" s="123" t="s">
         <v>299</v>
@@ -13909,7 +13954,7 @@
       <c r="F15" s="123"/>
       <c r="G15" s="123"/>
       <c r="H15" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I15" s="123" t="s">
         <v>300</v>
@@ -14144,7 +14189,7 @@
       <c r="F16" s="123"/>
       <c r="G16" s="123"/>
       <c r="H16" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I16" s="123" t="s">
         <v>301</v>
@@ -14380,7 +14425,7 @@
       <c r="F17" s="123"/>
       <c r="G17" s="123"/>
       <c r="H17" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I17" s="123" t="s">
         <v>302</v>
@@ -14616,7 +14661,7 @@
       <c r="F18" s="123"/>
       <c r="G18" s="123"/>
       <c r="H18" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I18" s="123" t="s">
         <v>303</v>
@@ -14852,7 +14897,7 @@
       <c r="F19" s="123"/>
       <c r="G19" s="123"/>
       <c r="H19" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I19" s="123" t="s">
         <v>304</v>
@@ -15088,7 +15133,7 @@
       <c r="F20" s="123"/>
       <c r="G20" s="123"/>
       <c r="H20" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I20" s="123" t="s">
         <v>305</v>
@@ -15324,7 +15369,7 @@
       <c r="F21" s="123"/>
       <c r="G21" s="123"/>
       <c r="H21" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I21" s="123" t="s">
         <v>306</v>
@@ -15560,7 +15605,7 @@
       <c r="F22" s="123"/>
       <c r="G22" s="123"/>
       <c r="H22" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I22" s="123" t="s">
         <v>307</v>
@@ -15796,7 +15841,7 @@
       <c r="F23" s="123"/>
       <c r="G23" s="123"/>
       <c r="H23" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I23" s="123" t="s">
         <v>308</v>
@@ -16032,7 +16077,7 @@
       <c r="F24" s="123"/>
       <c r="G24" s="123"/>
       <c r="H24" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I24" s="123" t="s">
         <v>309</v>
@@ -16267,7 +16312,7 @@
       <c r="F25" s="123"/>
       <c r="G25" s="123"/>
       <c r="H25" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I25" s="123" t="s">
         <v>310</v>
@@ -16502,7 +16547,7 @@
       <c r="F26" s="123"/>
       <c r="G26" s="123"/>
       <c r="H26" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I26" s="123" t="s">
         <v>311</v>
@@ -16738,7 +16783,7 @@
       <c r="F27" s="123"/>
       <c r="G27" s="123"/>
       <c r="H27" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I27" s="123" t="s">
         <v>312</v>
@@ -16974,7 +17019,7 @@
       <c r="F28" s="123"/>
       <c r="G28" s="123"/>
       <c r="H28" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I28" s="123" t="s">
         <v>313</v>
@@ -17210,7 +17255,7 @@
       <c r="F29" s="123"/>
       <c r="G29" s="123"/>
       <c r="H29" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I29" s="123" t="s">
         <v>314</v>
@@ -17446,7 +17491,7 @@
       <c r="F30" s="123"/>
       <c r="G30" s="123"/>
       <c r="H30" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I30" s="123" t="s">
         <v>315</v>
@@ -17682,7 +17727,7 @@
       <c r="F31" s="123"/>
       <c r="G31" s="123"/>
       <c r="H31" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I31" s="123" t="s">
         <v>316</v>
@@ -17918,7 +17963,7 @@
       <c r="F32" s="123"/>
       <c r="G32" s="123"/>
       <c r="H32" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I32" s="123" t="s">
         <v>317</v>
@@ -18154,7 +18199,7 @@
       <c r="F33" s="123"/>
       <c r="G33" s="123"/>
       <c r="H33" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I33" s="123" t="s">
         <v>318</v>
@@ -18198,7 +18243,7 @@
       <c r="F34" s="123"/>
       <c r="G34" s="123"/>
       <c r="H34" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I34" s="123" t="s">
         <v>319</v>
@@ -18242,7 +18287,7 @@
       <c r="F35" s="123"/>
       <c r="G35" s="123"/>
       <c r="H35" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I35" s="123" t="s">
         <v>320</v>
@@ -18478,7 +18523,7 @@
       <c r="F36" s="123"/>
       <c r="G36" s="123"/>
       <c r="H36" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I36" s="123" t="s">
         <v>321</v>
@@ -18714,7 +18759,7 @@
       <c r="F37" s="123"/>
       <c r="G37" s="123"/>
       <c r="H37" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I37" s="123" t="s">
         <v>322</v>
@@ -18950,7 +18995,7 @@
       <c r="F38" s="123"/>
       <c r="G38" s="123"/>
       <c r="H38" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I38" s="123" t="s">
         <v>323</v>
@@ -19186,7 +19231,7 @@
       <c r="F39" s="123"/>
       <c r="G39" s="123"/>
       <c r="H39" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I39" s="123" t="s">
         <v>324</v>
@@ -19422,7 +19467,7 @@
       <c r="F40" s="123"/>
       <c r="G40" s="123"/>
       <c r="H40" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I40" s="123" t="s">
         <v>325</v>
@@ -19658,7 +19703,7 @@
       <c r="F41" s="123"/>
       <c r="G41" s="123"/>
       <c r="H41" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I41" s="123" t="s">
         <v>326</v>
@@ -19894,7 +19939,7 @@
       <c r="F42" s="123"/>
       <c r="G42" s="123"/>
       <c r="H42" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I42" s="123" t="s">
         <v>327</v>
@@ -19932,7 +19977,7 @@
       <c r="F43" s="116"/>
       <c r="G43" s="116"/>
       <c r="H43" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I43" s="150" t="s">
         <v>51</v>
@@ -19970,7 +20015,7 @@
       <c r="F44" s="116"/>
       <c r="G44" s="116"/>
       <c r="H44" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I44" s="124" t="s">
         <v>52</v>
@@ -20008,7 +20053,7 @@
       <c r="F45" s="116"/>
       <c r="G45" s="116"/>
       <c r="H45" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I45" s="124" t="s">
         <v>53</v>
@@ -20046,7 +20091,7 @@
       <c r="F46" s="116"/>
       <c r="G46" s="116"/>
       <c r="H46" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I46" s="124" t="s">
         <v>54</v>
@@ -20086,7 +20131,7 @@
       <c r="F47" s="116"/>
       <c r="G47" s="116"/>
       <c r="H47" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I47" s="124" t="s">
         <v>55</v>
@@ -20122,7 +20167,7 @@
       <c r="F48" s="122"/>
       <c r="G48" s="122"/>
       <c r="H48" s="123" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I48" s="124" t="s">
         <v>56</v>
@@ -20527,7 +20572,7 @@
         <v>418</v>
       </c>
       <c r="J3" s="171" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="K3" s="123"/>
       <c r="L3" s="171" t="s">
@@ -20537,7 +20582,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="124" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="O3" s="124"/>
       <c r="P3" s="126"/>
@@ -22709,7 +22754,7 @@
         <v>32</v>
       </c>
       <c r="N13" s="123" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="O13" s="123"/>
       <c r="P13" s="147"/>
@@ -22949,7 +22994,7 @@
         <v>32</v>
       </c>
       <c r="N14" s="123" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="O14" s="123"/>
       <c r="P14" s="147"/>
@@ -26505,7 +26550,7 @@
         <v>32</v>
       </c>
       <c r="N29" s="123" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="O29" s="123"/>
       <c r="P29" s="147"/>
@@ -26981,7 +27026,7 @@
         <v>32</v>
       </c>
       <c r="N31" s="123" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="O31" s="123"/>
       <c r="P31" s="147"/>
@@ -27221,7 +27266,7 @@
         <v>32</v>
       </c>
       <c r="N32" s="123" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="O32" s="123"/>
       <c r="P32" s="147"/>
@@ -33374,9 +33419,9 @@
   </sheetPr>
   <dimension ref="A1:HF20"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -33752,7 +33797,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="123" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="O3" s="123"/>
       <c r="P3" s="147"/>
@@ -34456,7 +34501,7 @@
         <v>403</v>
       </c>
       <c r="J6" s="123" t="s">
-        <v>416</v>
+        <v>276</v>
       </c>
       <c r="K6" s="123" t="s">
         <v>416</v>
@@ -35872,7 +35917,7 @@
         <v>409</v>
       </c>
       <c r="J12" s="123" t="s">
-        <v>416</v>
+        <v>276</v>
       </c>
       <c r="K12" s="123" t="s">
         <v>416</v>
@@ -36804,16 +36849,16 @@
   </sheetPr>
   <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" style="190" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="190" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.7109375" customWidth="1"/>
@@ -36909,10 +36954,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="193" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C2" s="163" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D2" s="164"/>
       <c r="E2" s="164"/>
@@ -36975,7 +37020,7 @@
         <v>418</v>
       </c>
       <c r="J3" s="171" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="K3" s="171"/>
       <c r="L3" s="172" t="s">
@@ -36985,7 +37030,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="124" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="O3" s="124"/>
       <c r="P3" s="126"/>
@@ -36998,63 +37043,63 @@
       <c r="U3" s="124"/>
       <c r="V3" s="123"/>
     </row>
-    <row r="4" spans="1:22" outlineLevel="1">
-      <c r="A4" s="169" t="s">
+    <row r="4" spans="1:22" s="215" customFormat="1" outlineLevel="1">
+      <c r="A4" s="207" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="196" t="s">
-        <v>556</v>
-      </c>
-      <c r="C4" s="124" t="s">
-        <v>557</v>
-      </c>
-      <c r="D4" s="123" t="s">
+      <c r="B4" s="208" t="s">
+        <v>569</v>
+      </c>
+      <c r="C4" s="209" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="210" t="s">
         <v>451</v>
       </c>
       <c r="E4" s="192" t="s">
         <v>502</v>
       </c>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124" t="s">
+      <c r="F4" s="209"/>
+      <c r="G4" s="209"/>
+      <c r="H4" s="209" t="s">
         <v>501</v>
       </c>
-      <c r="I4" s="123" t="s">
+      <c r="I4" s="210" t="s">
         <v>451</v>
       </c>
-      <c r="J4" s="123" t="s">
+      <c r="J4" s="210" t="s">
         <v>504</v>
       </c>
-      <c r="K4" s="123" t="s">
+      <c r="K4" s="210" t="s">
         <v>504</v>
       </c>
-      <c r="L4" s="172" t="s">
+      <c r="L4" s="211" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="200" t="s">
+      <c r="M4" s="212" t="s">
         <v>32</v>
       </c>
       <c r="N4" s="192" t="s">
         <v>502</v>
       </c>
-      <c r="O4" s="124"/>
-      <c r="P4" s="126"/>
-      <c r="Q4" s="126"/>
-      <c r="R4" s="201"/>
-      <c r="S4" s="147"/>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="123"/>
+      <c r="O4" s="209"/>
+      <c r="P4" s="212"/>
+      <c r="Q4" s="212"/>
+      <c r="R4" s="213"/>
+      <c r="S4" s="214"/>
+      <c r="T4" s="209"/>
+      <c r="U4" s="209"/>
+      <c r="V4" s="210"/>
     </row>
     <row r="5" spans="1:22" outlineLevel="1">
       <c r="A5" s="169" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D5" s="123" t="s">
         <v>452</v>
@@ -37093,10 +37138,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D6" s="123" t="s">
         <v>453</v>
@@ -37141,10 +37186,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D7" s="123" t="s">
         <v>454</v>
@@ -37185,10 +37230,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C8" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D8" s="123" t="s">
         <v>455</v>
@@ -37229,10 +37274,10 @@
         <v>22</v>
       </c>
       <c r="B9" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C9" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D9" s="123" t="s">
         <v>456</v>
@@ -37273,10 +37318,10 @@
         <v>22</v>
       </c>
       <c r="B10" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C10" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D10" s="123" t="s">
         <v>457</v>
@@ -37317,10 +37362,10 @@
         <v>22</v>
       </c>
       <c r="B11" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C11" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D11" s="123" t="s">
         <v>458</v>
@@ -37365,10 +37410,10 @@
         <v>22</v>
       </c>
       <c r="B12" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C12" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D12" s="123" t="s">
         <v>459</v>
@@ -37413,10 +37458,10 @@
         <v>22</v>
       </c>
       <c r="B13" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C13" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D13" s="123" t="s">
         <v>460</v>
@@ -37457,10 +37502,10 @@
         <v>22</v>
       </c>
       <c r="B14" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C14" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D14" s="123" t="s">
         <v>461</v>
@@ -37501,10 +37546,10 @@
         <v>22</v>
       </c>
       <c r="B15" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C15" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D15" s="123" t="s">
         <v>462</v>
@@ -37545,10 +37590,10 @@
         <v>22</v>
       </c>
       <c r="B16" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C16" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D16" s="123" t="s">
         <v>463</v>
@@ -37589,10 +37634,10 @@
         <v>22</v>
       </c>
       <c r="B17" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C17" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D17" s="123" t="s">
         <v>464</v>
@@ -37633,10 +37678,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D18" s="123" t="s">
         <v>465</v>
@@ -37677,10 +37722,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C19" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D19" s="123" t="s">
         <v>466</v>
@@ -37721,10 +37766,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C20" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D20" s="123" t="s">
         <v>467</v>
@@ -37765,10 +37810,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C21" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D21" s="123" t="s">
         <v>468</v>
@@ -37809,10 +37854,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C22" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D22" s="123" t="s">
         <v>469</v>
@@ -37853,10 +37898,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C23" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D23" s="123" t="s">
         <v>470</v>
@@ -37897,10 +37942,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C24" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D24" s="123" t="s">
         <v>471</v>
@@ -37941,10 +37986,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C25" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D25" s="123" t="s">
         <v>472</v>
@@ -37985,10 +38030,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C26" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D26" s="123" t="s">
         <v>473</v>
@@ -38029,10 +38074,10 @@
         <v>22</v>
       </c>
       <c r="B27" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C27" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D27" s="123" t="s">
         <v>474</v>
@@ -38073,10 +38118,10 @@
         <v>22</v>
       </c>
       <c r="B28" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C28" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D28" s="123" t="s">
         <v>475</v>
@@ -38117,10 +38162,10 @@
         <v>22</v>
       </c>
       <c r="B29" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C29" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D29" s="123" t="s">
         <v>476</v>
@@ -38161,10 +38206,10 @@
         <v>22</v>
       </c>
       <c r="B30" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C30" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D30" s="123" t="s">
         <v>477</v>
@@ -38205,10 +38250,10 @@
         <v>22</v>
       </c>
       <c r="B31" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C31" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D31" s="123" t="s">
         <v>478</v>
@@ -38249,10 +38294,10 @@
         <v>22</v>
       </c>
       <c r="B32" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C32" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D32" s="123" t="s">
         <v>479</v>
@@ -38293,10 +38338,10 @@
         <v>22</v>
       </c>
       <c r="B33" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C33" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D33" s="123" t="s">
         <v>480</v>
@@ -38337,10 +38382,10 @@
         <v>22</v>
       </c>
       <c r="B34" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C34" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D34" s="123" t="s">
         <v>481</v>
@@ -38381,10 +38426,10 @@
         <v>22</v>
       </c>
       <c r="B35" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C35" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D35" s="123" t="s">
         <v>482</v>
@@ -38425,10 +38470,10 @@
         <v>22</v>
       </c>
       <c r="B36" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C36" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D36" s="123" t="s">
         <v>483</v>
@@ -38469,10 +38514,10 @@
         <v>22</v>
       </c>
       <c r="B37" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C37" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D37" s="123" t="s">
         <v>484</v>
@@ -38513,10 +38558,10 @@
         <v>22</v>
       </c>
       <c r="B38" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C38" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D38" s="123" t="s">
         <v>485</v>
@@ -38557,10 +38602,10 @@
         <v>22</v>
       </c>
       <c r="B39" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C39" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D39" s="123" t="s">
         <v>486</v>
@@ -38601,13 +38646,13 @@
         <v>22</v>
       </c>
       <c r="B40" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C40" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D40" s="123" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E40" s="124"/>
       <c r="F40" s="124"/>
@@ -38616,7 +38661,7 @@
         <v>501</v>
       </c>
       <c r="I40" s="123" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="J40" s="123" t="s">
         <v>110</v>
@@ -38645,10 +38690,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C41" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D41" s="123" t="s">
         <v>487</v>
@@ -38689,10 +38734,10 @@
         <v>22</v>
       </c>
       <c r="B42" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C42" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D42" s="123" t="s">
         <v>488</v>
@@ -38733,10 +38778,10 @@
         <v>22</v>
       </c>
       <c r="B43" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C43" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D43" s="123" t="s">
         <v>489</v>
@@ -38777,10 +38822,10 @@
         <v>22</v>
       </c>
       <c r="B44" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C44" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D44" s="123" t="s">
         <v>490</v>
@@ -38825,10 +38870,10 @@
         <v>22</v>
       </c>
       <c r="B45" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C45" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D45" s="123" t="s">
         <v>491</v>
@@ -38873,10 +38918,10 @@
         <v>22</v>
       </c>
       <c r="B46" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C46" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D46" s="123" t="s">
         <v>492</v>
@@ -38917,10 +38962,10 @@
         <v>22</v>
       </c>
       <c r="B47" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C47" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D47" s="123" t="s">
         <v>493</v>
@@ -38965,10 +39010,10 @@
         <v>22</v>
       </c>
       <c r="B48" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C48" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D48" s="123" t="s">
         <v>494</v>
@@ -39009,10 +39054,10 @@
         <v>22</v>
       </c>
       <c r="B49" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C49" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D49" s="123" t="s">
         <v>495</v>
@@ -39053,10 +39098,10 @@
         <v>22</v>
       </c>
       <c r="B50" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C50" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D50" s="123" t="s">
         <v>496</v>
@@ -39097,10 +39142,10 @@
         <v>22</v>
       </c>
       <c r="B51" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C51" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D51" s="123" t="s">
         <v>497</v>
@@ -39141,10 +39186,10 @@
         <v>22</v>
       </c>
       <c r="B52" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C52" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D52" s="123" t="s">
         <v>498</v>
@@ -39185,10 +39230,10 @@
         <v>22</v>
       </c>
       <c r="B53" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C53" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D53" s="123" t="s">
         <v>499</v>
@@ -39229,10 +39274,10 @@
         <v>22</v>
       </c>
       <c r="B54" s="196" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="C54" s="124" t="s">
-        <v>557</v>
+        <v>259</v>
       </c>
       <c r="D54" s="123" t="s">
         <v>500</v>
@@ -39686,7 +39731,7 @@
         <v>418</v>
       </c>
       <c r="J3" s="171" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="K3" s="123"/>
       <c r="L3" s="171" t="s">
@@ -39696,7 +39741,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="124" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="O3" s="124"/>
       <c r="P3" s="126"/>
@@ -40181,12 +40226,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -40282,7 +40327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="133" customFormat="1" ht="30" collapsed="1">
+    <row r="2" spans="1:22" s="133" customFormat="1" ht="30">
       <c r="A2" s="168" t="s">
         <v>22</v>
       </c>
@@ -40313,23 +40358,23 @@
         <v>31</v>
       </c>
       <c r="P2" s="167" t="str">
-        <f>IF(COUNTIF(P3:P27,"Y")&gt;0,"Y","N")</f>
+        <f>IF(COUNTIF(P3:P30,"Y")&gt;0,"Y","N")</f>
         <v>N</v>
       </c>
       <c r="Q2" s="167" t="str">
-        <f>IF(COUNTIF(Q3:Q27,"Y")&gt;0,"Y","N")</f>
+        <f>IF(COUNTIF(Q3:Q30,"Y")&gt;0,"Y","N")</f>
         <v>N</v>
       </c>
       <c r="R2" s="167" t="str">
-        <f>IF(COUNTIF(R3:R27,"Y")&gt;0,"Y","N")</f>
+        <f>IF(COUNTIF(R3:R30,"Y")&gt;0,"Y","N")</f>
         <v>Y</v>
       </c>
       <c r="S2" s="167" t="str">
-        <f>IF(COUNTIF(S3:S27,"Y")&gt;0,"Y","N")</f>
+        <f>IF(COUNTIF(S3:S30,"Y")&gt;0,"Y","N")</f>
         <v>N</v>
       </c>
       <c r="T2" s="168" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="U2" s="181" t="s">
         <v>390</v>
@@ -40338,39 +40383,31 @@
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="169" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="183" t="s">
-        <v>429</v>
-      </c>
-      <c r="C3" s="124" t="s">
-        <v>430</v>
-      </c>
-      <c r="D3" s="123" t="s">
-        <v>432</v>
-      </c>
-      <c r="E3" s="124"/>
+    <row r="3" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A3" s="169"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124" t="s">
+        <v>571</v>
+      </c>
       <c r="F3" s="124"/>
       <c r="G3" s="124"/>
       <c r="H3" s="124" t="s">
         <v>516</v>
       </c>
       <c r="I3" s="123" t="s">
-        <v>432</v>
+        <v>572</v>
       </c>
       <c r="J3" s="123" t="s">
-        <v>275</v>
-      </c>
-      <c r="K3" s="123" t="s">
-        <v>275</v>
-      </c>
-      <c r="L3" s="123" t="s">
-        <v>59</v>
+        <v>570</v>
+      </c>
+      <c r="K3" s="123"/>
+      <c r="L3" s="151" t="s">
+        <v>58</v>
       </c>
       <c r="M3" s="200" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="N3" s="124"/>
       <c r="O3" s="125"/>
@@ -40382,7 +40419,7 @@
       <c r="U3" s="124"/>
       <c r="V3" s="123"/>
     </row>
-    <row r="4" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="4" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A4" s="169" t="s">
         <v>22</v>
       </c>
@@ -40393,7 +40430,7 @@
         <v>430</v>
       </c>
       <c r="D4" s="123" t="s">
-        <v>517</v>
+        <v>432</v>
       </c>
       <c r="E4" s="124"/>
       <c r="F4" s="124"/>
@@ -40402,13 +40439,13 @@
         <v>516</v>
       </c>
       <c r="I4" s="123" t="s">
-        <v>517</v>
+        <v>432</v>
       </c>
       <c r="J4" s="123" t="s">
-        <v>64</v>
+        <v>275</v>
       </c>
       <c r="K4" s="123" t="s">
-        <v>64</v>
+        <v>275</v>
       </c>
       <c r="L4" s="123" t="s">
         <v>59</v>
@@ -40416,21 +40453,17 @@
       <c r="M4" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="124" t="s">
-        <v>529</v>
-      </c>
+      <c r="N4" s="124"/>
       <c r="O4" s="125"/>
       <c r="P4" s="124"/>
       <c r="Q4" s="126"/>
-      <c r="R4" s="126" t="s">
-        <v>32</v>
-      </c>
+      <c r="R4" s="126"/>
       <c r="S4" s="126"/>
       <c r="T4" s="124"/>
       <c r="U4" s="124"/>
       <c r="V4" s="123"/>
     </row>
-    <row r="5" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="5" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A5" s="169" t="s">
         <v>22</v>
       </c>
@@ -40441,7 +40474,7 @@
         <v>430</v>
       </c>
       <c r="D5" s="123" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E5" s="124"/>
       <c r="F5" s="124"/>
@@ -40450,7 +40483,7 @@
         <v>516</v>
       </c>
       <c r="I5" s="123" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J5" s="123" t="s">
         <v>64</v>
@@ -40464,17 +40497,21 @@
       <c r="M5" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="123"/>
+      <c r="N5" s="124" t="s">
+        <v>528</v>
+      </c>
       <c r="O5" s="125"/>
       <c r="P5" s="124"/>
       <c r="Q5" s="126"/>
-      <c r="R5" s="147"/>
+      <c r="R5" s="126" t="s">
+        <v>32</v>
+      </c>
       <c r="S5" s="126"/>
       <c r="T5" s="124"/>
       <c r="U5" s="124"/>
       <c r="V5" s="123"/>
     </row>
-    <row r="6" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="6" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A6" s="169" t="s">
         <v>22</v>
       </c>
@@ -40485,7 +40522,7 @@
         <v>430</v>
       </c>
       <c r="D6" s="123" t="s">
-        <v>437</v>
+        <v>518</v>
       </c>
       <c r="E6" s="124"/>
       <c r="F6" s="124"/>
@@ -40494,13 +40531,13 @@
         <v>516</v>
       </c>
       <c r="I6" s="123" t="s">
-        <v>437</v>
+        <v>518</v>
       </c>
       <c r="J6" s="123" t="s">
-        <v>276</v>
+        <v>64</v>
       </c>
       <c r="K6" s="123" t="s">
-        <v>276</v>
+        <v>64</v>
       </c>
       <c r="L6" s="123" t="s">
         <v>59</v>
@@ -40518,7 +40555,7 @@
       <c r="U6" s="124"/>
       <c r="V6" s="123"/>
     </row>
-    <row r="7" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="7" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A7" s="169" t="s">
         <v>22</v>
       </c>
@@ -40529,24 +40566,22 @@
         <v>430</v>
       </c>
       <c r="D7" s="123" t="s">
-        <v>519</v>
-      </c>
-      <c r="E7" s="124" t="s">
-        <v>438</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="E7" s="124"/>
       <c r="F7" s="124"/>
       <c r="G7" s="124"/>
       <c r="H7" s="124" t="s">
         <v>516</v>
       </c>
       <c r="I7" s="123" t="s">
-        <v>519</v>
+        <v>437</v>
       </c>
       <c r="J7" s="123" t="s">
-        <v>114</v>
+        <v>276</v>
       </c>
       <c r="K7" s="123" t="s">
-        <v>114</v>
+        <v>276</v>
       </c>
       <c r="L7" s="123" t="s">
         <v>59</v>
@@ -40554,19 +40589,17 @@
       <c r="M7" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="124" t="s">
-        <v>439</v>
-      </c>
+      <c r="N7" s="123"/>
       <c r="O7" s="125"/>
       <c r="P7" s="124"/>
       <c r="Q7" s="126"/>
-      <c r="R7" s="126"/>
+      <c r="R7" s="147"/>
       <c r="S7" s="126"/>
       <c r="T7" s="124"/>
       <c r="U7" s="124"/>
       <c r="V7" s="123"/>
     </row>
-    <row r="8" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="8" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A8" s="169" t="s">
         <v>22</v>
       </c>
@@ -40577,10 +40610,10 @@
         <v>430</v>
       </c>
       <c r="D8" s="123" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E8" s="124" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F8" s="124"/>
       <c r="G8" s="124"/>
@@ -40588,13 +40621,13 @@
         <v>516</v>
       </c>
       <c r="I8" s="123" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J8" s="123" t="s">
-        <v>530</v>
+        <v>114</v>
       </c>
       <c r="K8" s="123" t="s">
-        <v>530</v>
+        <v>114</v>
       </c>
       <c r="L8" s="123" t="s">
         <v>59</v>
@@ -40602,7 +40635,9 @@
       <c r="M8" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="124"/>
+      <c r="N8" s="124" t="s">
+        <v>439</v>
+      </c>
       <c r="O8" s="125"/>
       <c r="P8" s="124"/>
       <c r="Q8" s="126"/>
@@ -40612,7 +40647,7 @@
       <c r="U8" s="124"/>
       <c r="V8" s="123"/>
     </row>
-    <row r="9" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="9" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A9" s="169" t="s">
         <v>22</v>
       </c>
@@ -40623,22 +40658,24 @@
         <v>430</v>
       </c>
       <c r="D9" s="123" t="s">
-        <v>441</v>
-      </c>
-      <c r="E9" s="124"/>
+        <v>520</v>
+      </c>
+      <c r="E9" s="124" t="s">
+        <v>440</v>
+      </c>
       <c r="F9" s="124"/>
       <c r="G9" s="124"/>
       <c r="H9" s="124" t="s">
         <v>516</v>
       </c>
       <c r="I9" s="123" t="s">
-        <v>441</v>
+        <v>520</v>
       </c>
       <c r="J9" s="123" t="s">
-        <v>449</v>
+        <v>529</v>
       </c>
       <c r="K9" s="123" t="s">
-        <v>449</v>
+        <v>529</v>
       </c>
       <c r="L9" s="123" t="s">
         <v>59</v>
@@ -40656,7 +40693,7 @@
       <c r="U9" s="124"/>
       <c r="V9" s="123"/>
     </row>
-    <row r="10" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="10" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A10" s="169" t="s">
         <v>22</v>
       </c>
@@ -40667,7 +40704,7 @@
         <v>430</v>
       </c>
       <c r="D10" s="123" t="s">
-        <v>521</v>
+        <v>441</v>
       </c>
       <c r="E10" s="124"/>
       <c r="F10" s="124"/>
@@ -40676,7 +40713,7 @@
         <v>516</v>
       </c>
       <c r="I10" s="123" t="s">
-        <v>521</v>
+        <v>441</v>
       </c>
       <c r="J10" s="123" t="s">
         <v>449</v>
@@ -40700,7 +40737,7 @@
       <c r="U10" s="124"/>
       <c r="V10" s="123"/>
     </row>
-    <row r="11" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="11" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A11" s="169" t="s">
         <v>22</v>
       </c>
@@ -40711,7 +40748,7 @@
         <v>430</v>
       </c>
       <c r="D11" s="123" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E11" s="124"/>
       <c r="F11" s="124"/>
@@ -40720,7 +40757,7 @@
         <v>516</v>
       </c>
       <c r="I11" s="123" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J11" s="123" t="s">
         <v>449</v>
@@ -40744,7 +40781,7 @@
       <c r="U11" s="124"/>
       <c r="V11" s="123"/>
     </row>
-    <row r="12" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="12" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A12" s="169" t="s">
         <v>22</v>
       </c>
@@ -40755,7 +40792,7 @@
         <v>430</v>
       </c>
       <c r="D12" s="123" t="s">
-        <v>433</v>
+        <v>522</v>
       </c>
       <c r="E12" s="124"/>
       <c r="F12" s="124"/>
@@ -40764,13 +40801,13 @@
         <v>516</v>
       </c>
       <c r="I12" s="123" t="s">
-        <v>433</v>
+        <v>522</v>
       </c>
       <c r="J12" s="123" t="s">
-        <v>260</v>
+        <v>449</v>
       </c>
       <c r="K12" s="123" t="s">
-        <v>260</v>
+        <v>449</v>
       </c>
       <c r="L12" s="123" t="s">
         <v>59</v>
@@ -40778,21 +40815,17 @@
       <c r="M12" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="N12" s="124" t="s">
-        <v>434</v>
-      </c>
+      <c r="N12" s="124"/>
       <c r="O12" s="125"/>
       <c r="P12" s="124"/>
       <c r="Q12" s="126"/>
-      <c r="R12" s="126" t="s">
-        <v>32</v>
-      </c>
+      <c r="R12" s="126"/>
       <c r="S12" s="126"/>
       <c r="T12" s="124"/>
       <c r="U12" s="124"/>
       <c r="V12" s="123"/>
     </row>
-    <row r="13" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="13" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A13" s="169" t="s">
         <v>22</v>
       </c>
@@ -40803,7 +40836,7 @@
         <v>430</v>
       </c>
       <c r="D13" s="123" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E13" s="124"/>
       <c r="F13" s="124"/>
@@ -40812,13 +40845,13 @@
         <v>516</v>
       </c>
       <c r="I13" s="123" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J13" s="123" t="s">
-        <v>109</v>
+        <v>260</v>
       </c>
       <c r="K13" s="123" t="s">
-        <v>109</v>
+        <v>260</v>
       </c>
       <c r="L13" s="123" t="s">
         <v>59</v>
@@ -40827,7 +40860,7 @@
         <v>32</v>
       </c>
       <c r="N13" s="124" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="O13" s="125"/>
       <c r="P13" s="124"/>
@@ -40840,7 +40873,7 @@
       <c r="U13" s="124"/>
       <c r="V13" s="123"/>
     </row>
-    <row r="14" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="14" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A14" s="169" t="s">
         <v>22</v>
       </c>
@@ -40851,22 +40884,22 @@
         <v>430</v>
       </c>
       <c r="D14" s="123" t="s">
-        <v>523</v>
-      </c>
-      <c r="E14" s="123"/>
+        <v>435</v>
+      </c>
+      <c r="E14" s="124"/>
       <c r="F14" s="124"/>
       <c r="G14" s="124"/>
       <c r="H14" s="124" t="s">
         <v>516</v>
       </c>
       <c r="I14" s="123" t="s">
-        <v>523</v>
+        <v>435</v>
       </c>
       <c r="J14" s="123" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K14" s="123" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L14" s="123" t="s">
         <v>59</v>
@@ -40874,17 +40907,21 @@
       <c r="M14" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="N14" s="123"/>
+      <c r="N14" s="124" t="s">
+        <v>436</v>
+      </c>
       <c r="O14" s="125"/>
       <c r="P14" s="124"/>
       <c r="Q14" s="126"/>
-      <c r="R14" s="126"/>
+      <c r="R14" s="126" t="s">
+        <v>32</v>
+      </c>
       <c r="S14" s="126"/>
       <c r="T14" s="124"/>
       <c r="U14" s="124"/>
       <c r="V14" s="123"/>
     </row>
-    <row r="15" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="15" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A15" s="169" t="s">
         <v>22</v>
       </c>
@@ -40895,7 +40932,7 @@
         <v>430</v>
       </c>
       <c r="D15" s="123" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E15" s="123"/>
       <c r="F15" s="124"/>
@@ -40904,7 +40941,7 @@
         <v>516</v>
       </c>
       <c r="I15" s="123" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J15" s="123" t="s">
         <v>110</v>
@@ -40918,7 +40955,7 @@
       <c r="M15" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="N15" s="124"/>
+      <c r="N15" s="123"/>
       <c r="O15" s="125"/>
       <c r="P15" s="124"/>
       <c r="Q15" s="126"/>
@@ -40928,7 +40965,7 @@
       <c r="U15" s="124"/>
       <c r="V15" s="123"/>
     </row>
-    <row r="16" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="16" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A16" s="169" t="s">
         <v>22</v>
       </c>
@@ -40939,22 +40976,22 @@
         <v>430</v>
       </c>
       <c r="D16" s="123" t="s">
-        <v>525</v>
-      </c>
-      <c r="E16" s="124"/>
+        <v>524</v>
+      </c>
+      <c r="E16" s="123"/>
       <c r="F16" s="124"/>
       <c r="G16" s="124"/>
       <c r="H16" s="124" t="s">
         <v>516</v>
       </c>
       <c r="I16" s="123" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J16" s="123" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="K16" s="123" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="L16" s="123" t="s">
         <v>59</v>
@@ -40972,7 +41009,7 @@
       <c r="U16" s="124"/>
       <c r="V16" s="123"/>
     </row>
-    <row r="17" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="17" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A17" s="169" t="s">
         <v>22</v>
       </c>
@@ -40983,7 +41020,7 @@
         <v>430</v>
       </c>
       <c r="D17" s="123" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E17" s="124"/>
       <c r="F17" s="124"/>
@@ -40992,7 +41029,7 @@
         <v>516</v>
       </c>
       <c r="I17" s="123" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J17" s="123" t="s">
         <v>61</v>
@@ -41016,7 +41053,7 @@
       <c r="U17" s="124"/>
       <c r="V17" s="123"/>
     </row>
-    <row r="18" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="18" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A18" s="169" t="s">
         <v>22</v>
       </c>
@@ -41027,7 +41064,7 @@
         <v>430</v>
       </c>
       <c r="D18" s="123" t="s">
-        <v>442</v>
+        <v>526</v>
       </c>
       <c r="E18" s="124"/>
       <c r="F18" s="124"/>
@@ -41036,13 +41073,13 @@
         <v>516</v>
       </c>
       <c r="I18" s="123" t="s">
-        <v>442</v>
+        <v>526</v>
       </c>
       <c r="J18" s="123" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="K18" s="123" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="L18" s="123" t="s">
         <v>59</v>
@@ -41060,7 +41097,7 @@
       <c r="U18" s="124"/>
       <c r="V18" s="123"/>
     </row>
-    <row r="19" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="19" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A19" s="169" t="s">
         <v>22</v>
       </c>
@@ -41071,7 +41108,7 @@
         <v>430</v>
       </c>
       <c r="D19" s="123" t="s">
-        <v>527</v>
+        <v>442</v>
       </c>
       <c r="E19" s="124"/>
       <c r="F19" s="124"/>
@@ -41080,13 +41117,13 @@
         <v>516</v>
       </c>
       <c r="I19" s="123" t="s">
-        <v>527</v>
+        <v>442</v>
       </c>
       <c r="J19" s="123" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="K19" s="123" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="L19" s="123" t="s">
         <v>59</v>
@@ -41104,7 +41141,7 @@
       <c r="U19" s="124"/>
       <c r="V19" s="123"/>
     </row>
-    <row r="20" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="20" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A20" s="169" t="s">
         <v>22</v>
       </c>
@@ -41115,7 +41152,7 @@
         <v>430</v>
       </c>
       <c r="D20" s="123" t="s">
-        <v>443</v>
+        <v>527</v>
       </c>
       <c r="E20" s="124"/>
       <c r="F20" s="124"/>
@@ -41124,13 +41161,13 @@
         <v>516</v>
       </c>
       <c r="I20" s="123" t="s">
-        <v>443</v>
+        <v>527</v>
       </c>
       <c r="J20" s="123" t="s">
-        <v>275</v>
+        <v>115</v>
       </c>
       <c r="K20" s="123" t="s">
-        <v>275</v>
+        <v>115</v>
       </c>
       <c r="L20" s="123" t="s">
         <v>59</v>
@@ -41148,7 +41185,7 @@
       <c r="U20" s="124"/>
       <c r="V20" s="123"/>
     </row>
-    <row r="21" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="21" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A21" s="169" t="s">
         <v>22</v>
       </c>
@@ -41159,7 +41196,7 @@
         <v>430</v>
       </c>
       <c r="D21" s="123" t="s">
-        <v>528</v>
+        <v>443</v>
       </c>
       <c r="E21" s="124"/>
       <c r="F21" s="124"/>
@@ -41168,13 +41205,13 @@
         <v>516</v>
       </c>
       <c r="I21" s="123" t="s">
-        <v>528</v>
+        <v>443</v>
       </c>
       <c r="J21" s="123" t="s">
-        <v>110</v>
+        <v>275</v>
       </c>
       <c r="K21" s="123" t="s">
-        <v>110</v>
+        <v>275</v>
       </c>
       <c r="L21" s="123" t="s">
         <v>59</v>
@@ -41192,7 +41229,7 @@
       <c r="U21" s="124"/>
       <c r="V21" s="123"/>
     </row>
-    <row r="22" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="22" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A22" s="169" t="s">
         <v>22</v>
       </c>
@@ -41203,7 +41240,7 @@
         <v>430</v>
       </c>
       <c r="D22" s="123" t="s">
-        <v>444</v>
+        <v>573</v>
       </c>
       <c r="E22" s="124"/>
       <c r="F22" s="124"/>
@@ -41212,13 +41249,13 @@
         <v>516</v>
       </c>
       <c r="I22" s="123" t="s">
-        <v>444</v>
+        <v>573</v>
       </c>
       <c r="J22" s="123" t="s">
-        <v>276</v>
+        <v>110</v>
       </c>
       <c r="K22" s="123" t="s">
-        <v>276</v>
+        <v>110</v>
       </c>
       <c r="L22" s="123" t="s">
         <v>59</v>
@@ -41236,35 +41273,41 @@
       <c r="U22" s="124"/>
       <c r="V22" s="123"/>
     </row>
-    <row r="23" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A23" s="173"/>
-      <c r="B23" s="174"/>
-      <c r="C23" s="124"/>
-      <c r="D23" s="124"/>
-      <c r="E23" s="124" t="s">
-        <v>46</v>
-      </c>
+    <row r="23" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A23" s="169" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="183" t="s">
+        <v>429</v>
+      </c>
+      <c r="C23" s="124" t="s">
+        <v>430</v>
+      </c>
+      <c r="D23" s="123" t="s">
+        <v>568</v>
+      </c>
+      <c r="E23" s="124"/>
       <c r="F23" s="124"/>
       <c r="G23" s="124"/>
       <c r="H23" s="124" t="s">
         <v>516</v>
       </c>
-      <c r="I23" s="124" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="124" t="s">
-        <v>116</v>
-      </c>
-      <c r="K23" s="184"/>
-      <c r="L23" s="151" t="s">
-        <v>58</v>
+      <c r="I23" s="123" t="s">
+        <v>568</v>
+      </c>
+      <c r="J23" s="123" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="123" t="s">
+        <v>110</v>
+      </c>
+      <c r="L23" s="123" t="s">
+        <v>59</v>
       </c>
       <c r="M23" s="200" t="s">
-        <v>57</v>
-      </c>
-      <c r="N23" s="175" t="s">
-        <v>67</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N23" s="124"/>
       <c r="O23" s="125"/>
       <c r="P23" s="124"/>
       <c r="Q23" s="126"/>
@@ -41274,35 +41317,41 @@
       <c r="U23" s="124"/>
       <c r="V23" s="123"/>
     </row>
-    <row r="24" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A24" s="173"/>
-      <c r="B24" s="174"/>
-      <c r="C24" s="124"/>
-      <c r="D24" s="124"/>
-      <c r="E24" s="124" t="s">
-        <v>47</v>
-      </c>
+    <row r="24" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A24" s="169" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="183" t="s">
+        <v>429</v>
+      </c>
+      <c r="C24" s="124" t="s">
+        <v>430</v>
+      </c>
+      <c r="D24" s="123" t="s">
+        <v>444</v>
+      </c>
+      <c r="E24" s="124"/>
       <c r="F24" s="124"/>
       <c r="G24" s="124"/>
       <c r="H24" s="124" t="s">
         <v>516</v>
       </c>
-      <c r="I24" s="124" t="s">
-        <v>52</v>
-      </c>
-      <c r="J24" s="124" t="s">
-        <v>117</v>
-      </c>
-      <c r="K24" s="184"/>
-      <c r="L24" s="153" t="s">
-        <v>58</v>
+      <c r="I24" s="123" t="s">
+        <v>444</v>
+      </c>
+      <c r="J24" s="123" t="s">
+        <v>276</v>
+      </c>
+      <c r="K24" s="123" t="s">
+        <v>276</v>
+      </c>
+      <c r="L24" s="123" t="s">
+        <v>59</v>
       </c>
       <c r="M24" s="200" t="s">
-        <v>57</v>
-      </c>
-      <c r="N24" s="125" t="s">
-        <v>68</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N24" s="124"/>
       <c r="O24" s="125"/>
       <c r="P24" s="124"/>
       <c r="Q24" s="126"/>
@@ -41312,13 +41361,13 @@
       <c r="U24" s="124"/>
       <c r="V24" s="123"/>
     </row>
-    <row r="25" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="25" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A25" s="173"/>
       <c r="B25" s="174"/>
       <c r="C25" s="124"/>
       <c r="D25" s="124"/>
       <c r="E25" s="124" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F25" s="124"/>
       <c r="G25" s="124"/>
@@ -41326,20 +41375,20 @@
         <v>516</v>
       </c>
       <c r="I25" s="124" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J25" s="124" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K25" s="184"/>
-      <c r="L25" s="153" t="s">
+      <c r="L25" s="151" t="s">
         <v>58</v>
       </c>
       <c r="M25" s="200" t="s">
         <v>57</v>
       </c>
-      <c r="N25" s="127" t="s">
-        <v>69</v>
+      <c r="N25" s="175" t="s">
+        <v>67</v>
       </c>
       <c r="O25" s="125"/>
       <c r="P25" s="124"/>
@@ -41350,13 +41399,13 @@
       <c r="U25" s="124"/>
       <c r="V25" s="123"/>
     </row>
-    <row r="26" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="26" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A26" s="173"/>
       <c r="B26" s="174"/>
       <c r="C26" s="124"/>
       <c r="D26" s="124"/>
       <c r="E26" s="124" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F26" s="124"/>
       <c r="G26" s="124"/>
@@ -41364,10 +41413,10 @@
         <v>516</v>
       </c>
       <c r="I26" s="124" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J26" s="124" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K26" s="184"/>
       <c r="L26" s="153" t="s">
@@ -41376,8 +41425,8 @@
       <c r="M26" s="200" t="s">
         <v>57</v>
       </c>
-      <c r="N26" s="176" t="s">
-        <v>270</v>
+      <c r="N26" s="125" t="s">
+        <v>68</v>
       </c>
       <c r="O26" s="125"/>
       <c r="P26" s="124"/>
@@ -41388,13 +41437,13 @@
       <c r="U26" s="124"/>
       <c r="V26" s="123"/>
     </row>
-    <row r="27" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="27" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A27" s="173"/>
       <c r="B27" s="174"/>
       <c r="C27" s="124"/>
       <c r="D27" s="124"/>
       <c r="E27" s="124" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F27" s="124"/>
       <c r="G27" s="124"/>
@@ -41402,10 +41451,10 @@
         <v>516</v>
       </c>
       <c r="I27" s="124" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J27" s="124" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K27" s="184"/>
       <c r="L27" s="153" t="s">
@@ -41414,8 +41463,8 @@
       <c r="M27" s="200" t="s">
         <v>57</v>
       </c>
-      <c r="N27" s="177" t="s">
-        <v>71</v>
+      <c r="N27" s="127" t="s">
+        <v>69</v>
       </c>
       <c r="O27" s="125"/>
       <c r="P27" s="124"/>
@@ -41426,46 +41475,160 @@
       <c r="U27" s="124"/>
       <c r="V27" s="123"/>
     </row>
-    <row r="28" spans="1:22" ht="15" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="28" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
       <c r="A28" s="173"/>
       <c r="B28" s="174"/>
       <c r="C28" s="124"/>
       <c r="D28" s="124"/>
-      <c r="E28" s="124"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="122"/>
+      <c r="E28" s="124" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="124"/>
+      <c r="G28" s="124"/>
       <c r="H28" s="124" t="s">
         <v>516</v>
       </c>
       <c r="I28" s="124" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J28" s="124" t="s">
-        <v>118</v>
-      </c>
-      <c r="K28" s="124"/>
-      <c r="L28" s="125" t="s">
+        <v>114</v>
+      </c>
+      <c r="K28" s="184"/>
+      <c r="L28" s="153" t="s">
         <v>58</v>
       </c>
       <c r="M28" s="200" t="s">
         <v>57</v>
       </c>
-      <c r="N28" s="127" t="s">
+      <c r="N28" s="176" t="s">
+        <v>270</v>
+      </c>
+      <c r="O28" s="125"/>
+      <c r="P28" s="124"/>
+      <c r="Q28" s="126"/>
+      <c r="R28" s="126"/>
+      <c r="S28" s="126"/>
+      <c r="T28" s="124"/>
+      <c r="U28" s="124"/>
+      <c r="V28" s="123"/>
+    </row>
+    <row r="29" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A29" s="173"/>
+      <c r="B29" s="174"/>
+      <c r="C29" s="124"/>
+      <c r="D29" s="124"/>
+      <c r="E29" s="124" t="s">
+        <v>576</v>
+      </c>
+      <c r="F29" s="124"/>
+      <c r="G29" s="124"/>
+      <c r="H29" s="124" t="s">
+        <v>516</v>
+      </c>
+      <c r="I29" s="124" t="s">
+        <v>574</v>
+      </c>
+      <c r="J29" s="124" t="s">
+        <v>575</v>
+      </c>
+      <c r="K29" s="184"/>
+      <c r="L29" s="153" t="s">
+        <v>58</v>
+      </c>
+      <c r="M29" s="200" t="s">
+        <v>57</v>
+      </c>
+      <c r="N29" s="124" t="s">
+        <v>576</v>
+      </c>
+      <c r="O29" s="125"/>
+      <c r="P29" s="124"/>
+      <c r="Q29" s="126"/>
+      <c r="R29" s="126"/>
+      <c r="S29" s="126"/>
+      <c r="T29" s="124"/>
+      <c r="U29" s="124"/>
+      <c r="V29" s="123"/>
+    </row>
+    <row r="30" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A30" s="173"/>
+      <c r="B30" s="174"/>
+      <c r="C30" s="124"/>
+      <c r="D30" s="124"/>
+      <c r="E30" s="124" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="124"/>
+      <c r="G30" s="124"/>
+      <c r="H30" s="124" t="s">
+        <v>516</v>
+      </c>
+      <c r="I30" s="124" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="124" t="s">
+        <v>119</v>
+      </c>
+      <c r="K30" s="184"/>
+      <c r="L30" s="153" t="s">
+        <v>58</v>
+      </c>
+      <c r="M30" s="200" t="s">
+        <v>57</v>
+      </c>
+      <c r="N30" s="177" t="s">
+        <v>71</v>
+      </c>
+      <c r="O30" s="125"/>
+      <c r="P30" s="124"/>
+      <c r="Q30" s="126"/>
+      <c r="R30" s="126"/>
+      <c r="S30" s="126"/>
+      <c r="T30" s="124"/>
+      <c r="U30" s="124"/>
+      <c r="V30" s="123"/>
+    </row>
+    <row r="31" spans="1:22" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A31" s="173"/>
+      <c r="B31" s="174"/>
+      <c r="C31" s="124"/>
+      <c r="D31" s="124"/>
+      <c r="E31" s="124"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="122"/>
+      <c r="H31" s="124" t="s">
+        <v>516</v>
+      </c>
+      <c r="I31" s="124" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="124" t="s">
+        <v>118</v>
+      </c>
+      <c r="K31" s="124"/>
+      <c r="L31" s="125" t="s">
+        <v>58</v>
+      </c>
+      <c r="M31" s="200" t="s">
+        <v>57</v>
+      </c>
+      <c r="N31" s="127" t="s">
         <v>271</v>
       </c>
-      <c r="O28" s="122"/>
-      <c r="P28" s="120"/>
-      <c r="Q28" s="120"/>
-      <c r="R28" s="120"/>
-      <c r="S28" s="120"/>
-      <c r="T28" s="120"/>
-      <c r="U28" s="120"/>
-      <c r="V28" s="120"/>
+      <c r="O31" s="122"/>
+      <c r="P31" s="120"/>
+      <c r="Q31" s="120"/>
+      <c r="R31" s="120"/>
+      <c r="S31" s="120"/>
+      <c r="T31" s="120"/>
+      <c r="U31" s="120"/>
+      <c r="V31" s="120"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U28"/>
+  <autoFilter ref="A1:U31"/>
   <hyperlinks>
-    <hyperlink ref="N26" location="'File_Date Reference'!A1" display="Refer to logic in document in Sheet &quot;File_Date_Reference&quot; Case No. &quot;01&quot;"/>
+    <hyperlink ref="N28" location="'File_Date Reference'!A1" display="Refer to logic in document in Sheet &quot;File_Date_Reference&quot; Case No. &quot;01&quot;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -41482,7 +41645,7 @@
   </sheetPr>
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
@@ -41584,7 +41747,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="186" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C2" s="166" t="s">
         <v>259</v>
@@ -41598,7 +41761,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="203" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I2" s="166"/>
       <c r="J2" s="166"/>
@@ -41639,22 +41802,22 @@
         <v>22</v>
       </c>
       <c r="B3" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C3" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D3" s="123" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E3" s="124"/>
       <c r="F3" s="124"/>
       <c r="G3" s="124"/>
       <c r="H3" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I3" s="123" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="J3" s="123" t="s">
         <v>450</v>
@@ -41669,7 +41832,7 @@
         <v>32</v>
       </c>
       <c r="N3" s="124" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="O3" s="124"/>
       <c r="P3" s="126"/>
@@ -41687,22 +41850,22 @@
         <v>22</v>
       </c>
       <c r="B4" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C4" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D4" s="123" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E4" s="124"/>
       <c r="F4" s="124"/>
       <c r="G4" s="124"/>
       <c r="H4" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I4" s="123" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J4" s="123" t="s">
         <v>447</v>
@@ -41731,22 +41894,22 @@
         <v>22</v>
       </c>
       <c r="B5" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C5" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D5" s="123" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E5" s="124"/>
       <c r="F5" s="124"/>
       <c r="G5" s="124"/>
       <c r="H5" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I5" s="123" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J5" s="123" t="s">
         <v>448</v>
@@ -41775,22 +41938,22 @@
         <v>22</v>
       </c>
       <c r="B6" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C6" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D6" s="123" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E6" s="124"/>
       <c r="F6" s="124"/>
       <c r="G6" s="124"/>
       <c r="H6" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I6" s="123" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J6" s="123" t="s">
         <v>62</v>
@@ -41819,22 +41982,22 @@
         <v>22</v>
       </c>
       <c r="B7" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C7" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D7" s="123" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E7" s="124"/>
       <c r="F7" s="124"/>
       <c r="G7" s="124"/>
       <c r="H7" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I7" s="123" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J7" s="123" t="s">
         <v>279</v>
@@ -41863,22 +42026,22 @@
         <v>22</v>
       </c>
       <c r="B8" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C8" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D8" s="123" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E8" s="124"/>
       <c r="F8" s="124"/>
       <c r="G8" s="124"/>
       <c r="H8" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I8" s="123" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J8" s="123" t="s">
         <v>422</v>
@@ -41907,24 +42070,24 @@
         <v>22</v>
       </c>
       <c r="B9" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C9" s="124" t="s">
         <v>259</v>
       </c>
       <c r="D9" s="123" t="s">
+        <v>538</v>
+      </c>
+      <c r="E9" s="124" t="s">
         <v>539</v>
-      </c>
-      <c r="E9" s="124" t="s">
-        <v>540</v>
       </c>
       <c r="F9" s="124"/>
       <c r="G9" s="124"/>
       <c r="H9" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I9" s="123" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J9" s="123" t="s">
         <v>65</v>
@@ -41939,7 +42102,7 @@
         <v>32</v>
       </c>
       <c r="N9" s="124" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O9" s="124"/>
       <c r="P9" s="126"/>
@@ -41961,7 +42124,7 @@
       <c r="F10" s="124"/>
       <c r="G10" s="124"/>
       <c r="H10" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I10" s="124" t="s">
         <v>51</v>
@@ -41999,7 +42162,7 @@
       <c r="F11" s="124"/>
       <c r="G11" s="124"/>
       <c r="H11" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I11" s="124" t="s">
         <v>52</v>
@@ -42037,7 +42200,7 @@
       <c r="F12" s="124"/>
       <c r="G12" s="124"/>
       <c r="H12" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I12" s="124" t="s">
         <v>53</v>
@@ -42075,7 +42238,7 @@
       <c r="F13" s="124"/>
       <c r="G13" s="124"/>
       <c r="H13" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I13" s="124" t="s">
         <v>54</v>
@@ -42115,7 +42278,7 @@
       <c r="F14" s="124"/>
       <c r="G14" s="124"/>
       <c r="H14" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I14" s="124" t="s">
         <v>55</v>
@@ -42151,7 +42314,7 @@
       <c r="F15" s="122"/>
       <c r="G15" s="122"/>
       <c r="H15" s="170" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I15" s="124" t="s">
         <v>56</v>
@@ -42205,6 +42368,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C723A6D629A244B9035064CEA29699F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="439c1f6a0871fabbc20469cf751fc22a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5c6a5f84-dc80-404b-9608-a58c80d813cf" xmlns:ns3="fb15ab9c-5ce3-4966-97a0-841ffe55082a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3a0ba7a63f3f3ddebd5188756dbc3799" ns2:_="" ns3:_="">
     <xsd:import namespace="5c6a5f84-dc80-404b-9608-a58c80d813cf"/>
@@ -42421,15 +42593,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86484D21-336C-4699-B297-37FD20E87A03}">
   <ds:schemaRefs>
@@ -42440,6 +42603,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6CC5F60-7C71-49F9-855C-F002D6759E81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D51A253-8FCC-480C-8849-892D45D1BD92}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42456,12 +42627,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6CC5F60-7C71-49F9-855C-F002D6759E81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>